<commit_message>
add update to 3 files for update password function
</commit_message>
<xml_diff>
--- a/spec/PHP_Training_Task17060_APIFormat_Ver_0.1.0.xlsx
+++ b/spec/PHP_Training_Task17060_APIFormat_Ver_0.1.0.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="640" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="640" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="API List" sheetId="1" r:id="rId1"/>
     <sheet name="login" sheetId="13" r:id="rId2"/>
     <sheet name="regedit" sheetId="14" r:id="rId3"/>
+    <sheet name="updatepassword" sheetId="16" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="88">
   <si>
     <t>No</t>
   </si>
@@ -294,6 +295,27 @@
   </si>
   <si>
     <t>regedit</t>
+  </si>
+  <si>
+    <t>Update password</t>
+  </si>
+  <si>
+    <t>Old Password</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>New Password</t>
+  </si>
+  <si>
+    <t>Match Password</t>
+  </si>
+  <si>
+    <t>hgbkfjlads7389fhklfads2390</t>
+  </si>
+  <si>
+    <t>The API is used when user want to update password.</t>
   </si>
 </sst>
 </file>
@@ -306,7 +328,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -394,7 +415,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -551,8 +572,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="70">
+  <cellStyleXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -623,8 +653,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -711,6 +749,30 @@
     <xf numFmtId="49" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="37" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -741,26 +803,11 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="37" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="70">
+  <cellStyles count="78">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -811,6 +858,14 @@
     <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1010,6 +1065,178 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>540026</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>167311</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>629477</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>110435</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1365526" y="6009311"/>
+          <a:ext cx="10744751" cy="1721124"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="0" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="ＭＳ ゴシック"/>
+              <a:ea typeface="ＭＳ ゴシック"/>
+            </a:rPr>
+            <a:t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="ＭＳ ゴシック"/>
+              <a:ea typeface="ＭＳ ゴシック"/>
+            </a:rPr>
+            <a:t>&lt;response lang="vi" xml:lang="vi"&gt;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="ＭＳ ゴシック"/>
+              <a:ea typeface="ＭＳ ゴシック"/>
+            </a:rPr>
+            <a:t>    &lt;error&gt;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="ＭＳ ゴシック"/>
+              <a:ea typeface="ＭＳ ゴシック"/>
+            </a:rPr>
+            <a:t>        &lt;status&gt;200&lt;/status&gt;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="ＭＳ ゴシック"/>
+              <a:ea typeface="ＭＳ ゴシック"/>
+            </a:rPr>
+            <a:t>        &lt;message&gt;&lt;/message&gt;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="ＭＳ ゴシック"/>
+              <a:ea typeface="ＭＳ ゴシック"/>
+            </a:rPr>
+            <a:t>    &lt;/error&gt;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="ＭＳ ゴシック"/>
+              <a:ea typeface="ＭＳ ゴシック"/>
+            </a:rPr>
+            <a:t>    &lt;token&gt;346583hfh57ty4ig4&lt;/token&gt;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="ＭＳ ゴシック"/>
+              <a:ea typeface="ＭＳ ゴシック"/>
+            </a:rPr>
+            <a:t>&lt;/response&gt;</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1556,7 +1783,7 @@
       <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" s="67" t="s">
+      <c r="B3" s="54" t="s">
         <v>69</v>
       </c>
       <c r="C3" s="8" t="s">
@@ -1733,7 +1960,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O97"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="A20" sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
@@ -1814,15 +2043,15 @@
       <c r="B4" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="62" t="s">
+      <c r="C4" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="66"/>
-      <c r="E4" s="66"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="66"/>
-      <c r="I4" s="63"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="56"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
@@ -1835,15 +2064,15 @@
       <c r="B5" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="62" t="s">
+      <c r="C5" s="55" t="s">
         <v>63</v>
       </c>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
-      <c r="I5" s="63"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="56"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -1856,15 +2085,15 @@
       <c r="B6" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="62" t="s">
+      <c r="C6" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="66"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="66"/>
-      <c r="G6" s="66"/>
-      <c r="H6" s="66"/>
-      <c r="I6" s="63"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="59"/>
+      <c r="G6" s="59"/>
+      <c r="H6" s="59"/>
+      <c r="I6" s="56"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -1877,15 +2106,15 @@
       <c r="B7" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="62" t="s">
+      <c r="C7" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="66"/>
-      <c r="E7" s="66"/>
-      <c r="F7" s="66"/>
-      <c r="G7" s="66"/>
-      <c r="H7" s="66"/>
-      <c r="I7" s="63"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="59"/>
+      <c r="G7" s="59"/>
+      <c r="H7" s="59"/>
+      <c r="I7" s="56"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -1950,19 +2179,19 @@
     </row>
     <row r="11" spans="1:15" ht="20" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="61"/>
+      <c r="C11" s="69"/>
       <c r="D11" s="44"/>
       <c r="E11" s="44"/>
       <c r="F11" s="44"/>
       <c r="G11" s="44"/>
       <c r="H11" s="44"/>
       <c r="I11" s="44"/>
-      <c r="J11" s="57"/>
-      <c r="K11" s="57"/>
-      <c r="L11" s="57"/>
+      <c r="J11" s="65"/>
+      <c r="K11" s="65"/>
+      <c r="L11" s="65"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
@@ -1991,11 +2220,11 @@
       <c r="I12" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="J12" s="58" t="s">
+      <c r="J12" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="K12" s="58"/>
-      <c r="L12" s="58"/>
+      <c r="K12" s="66"/>
+      <c r="L12" s="66"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
@@ -2024,11 +2253,11 @@
       <c r="I13" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="J13" s="52" t="s">
+      <c r="J13" s="60" t="s">
         <v>49</v>
       </c>
-      <c r="K13" s="52"/>
-      <c r="L13" s="52"/>
+      <c r="K13" s="60"/>
+      <c r="L13" s="60"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
@@ -2057,11 +2286,11 @@
       <c r="I14" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="J14" s="52" t="s">
+      <c r="J14" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="K14" s="52"/>
-      <c r="L14" s="52"/>
+      <c r="K14" s="60"/>
+      <c r="L14" s="60"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
@@ -2085,11 +2314,11 @@
     </row>
     <row r="16" spans="1:15" s="19" customFormat="1" ht="20" customHeight="1">
       <c r="A16" s="11"/>
-      <c r="B16" s="59" t="s">
+      <c r="B16" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="59"/>
-      <c r="D16" s="59"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="67"/>
       <c r="E16" s="17"/>
       <c r="F16" s="18"/>
       <c r="G16" s="17"/>
@@ -2104,12 +2333,12 @@
     </row>
     <row r="17" spans="1:15" s="23" customFormat="1" ht="20" customHeight="1">
       <c r="A17" s="21"/>
-      <c r="B17" s="53" t="s">
+      <c r="B17" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="54"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="55"/>
+      <c r="C17" s="62"/>
+      <c r="D17" s="62"/>
+      <c r="E17" s="63"/>
       <c r="F17" s="22" t="s">
         <v>21</v>
       </c>
@@ -2298,10 +2527,10 @@
       <c r="A23" s="1"/>
       <c r="B23" s="31"/>
       <c r="C23" s="32"/>
-      <c r="D23" s="62" t="s">
+      <c r="D23" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="E23" s="63"/>
+      <c r="E23" s="56"/>
       <c r="F23" s="14" t="s">
         <v>59</v>
       </c>
@@ -2465,11 +2694,11 @@
     </row>
     <row r="32" spans="1:15" ht="20" customHeight="1">
       <c r="A32" s="1"/>
-      <c r="B32" s="56" t="s">
+      <c r="B32" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="56"/>
-      <c r="D32" s="56"/>
+      <c r="C32" s="64"/>
+      <c r="D32" s="64"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
@@ -2484,12 +2713,12 @@
     </row>
     <row r="33" spans="1:15" ht="20" customHeight="1">
       <c r="A33" s="1"/>
-      <c r="B33" s="53" t="s">
+      <c r="B33" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="C33" s="54"/>
-      <c r="D33" s="54"/>
-      <c r="E33" s="55"/>
+      <c r="C33" s="62"/>
+      <c r="D33" s="62"/>
+      <c r="E33" s="63"/>
       <c r="F33" s="22" t="s">
         <v>21</v>
       </c>
@@ -2693,11 +2922,11 @@
     </row>
     <row r="40" spans="1:15" ht="20" customHeight="1">
       <c r="A40" s="1"/>
-      <c r="B40" s="56" t="s">
+      <c r="B40" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="C40" s="56"/>
-      <c r="D40" s="56"/>
+      <c r="C40" s="64"/>
+      <c r="D40" s="64"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
@@ -2715,10 +2944,10 @@
       <c r="B41" s="38">
         <v>200</v>
       </c>
-      <c r="C41" s="62" t="s">
+      <c r="C41" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="D41" s="63"/>
+      <c r="D41" s="56"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
@@ -2736,10 +2965,10 @@
       <c r="B42" s="38">
         <v>401</v>
       </c>
-      <c r="C42" s="62" t="s">
+      <c r="C42" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="D42" s="63"/>
+      <c r="D42" s="56"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
@@ -2757,10 +2986,10 @@
       <c r="B43" s="45">
         <v>402</v>
       </c>
-      <c r="C43" s="62" t="s">
+      <c r="C43" s="55" t="s">
         <v>68</v>
       </c>
-      <c r="D43" s="63"/>
+      <c r="D43" s="56"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
@@ -2778,10 +3007,10 @@
       <c r="B44" s="39">
         <v>500</v>
       </c>
-      <c r="C44" s="64" t="s">
+      <c r="C44" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="D44" s="65"/>
+      <c r="D44" s="58"/>
       <c r="E44" s="34"/>
       <c r="F44" s="34"/>
       <c r="G44" s="34"/>
@@ -3697,14 +3926,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C4:I4"/>
-    <mergeCell ref="C5:I5"/>
-    <mergeCell ref="C6:I6"/>
-    <mergeCell ref="C7:I7"/>
-    <mergeCell ref="C43:D43"/>
     <mergeCell ref="J14:L14"/>
     <mergeCell ref="B33:E33"/>
     <mergeCell ref="B40:D40"/>
@@ -3716,6 +3937,14 @@
     <mergeCell ref="B32:D32"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="D23:E23"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="C5:I5"/>
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="C7:I7"/>
+    <mergeCell ref="C43:D43"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <hyperlinks>
@@ -3736,7 +3965,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O100"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A5" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="A29" sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
@@ -3817,15 +4048,15 @@
       <c r="B4" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="62" t="s">
+      <c r="C4" s="55" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="66"/>
-      <c r="E4" s="66"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="66"/>
-      <c r="I4" s="63"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="56"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
@@ -3838,15 +4069,15 @@
       <c r="B5" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="62" t="s">
+      <c r="C5" s="55" t="s">
         <v>70</v>
       </c>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
-      <c r="I5" s="63"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="56"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -3859,15 +4090,15 @@
       <c r="B6" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="62" t="s">
+      <c r="C6" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="66"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="66"/>
-      <c r="G6" s="66"/>
-      <c r="H6" s="66"/>
-      <c r="I6" s="63"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="59"/>
+      <c r="G6" s="59"/>
+      <c r="H6" s="59"/>
+      <c r="I6" s="56"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -3880,15 +4111,15 @@
       <c r="B7" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="62" t="s">
+      <c r="C7" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="66"/>
-      <c r="E7" s="66"/>
-      <c r="F7" s="66"/>
-      <c r="G7" s="66"/>
-      <c r="H7" s="66"/>
-      <c r="I7" s="63"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="59"/>
+      <c r="G7" s="59"/>
+      <c r="H7" s="59"/>
+      <c r="I7" s="56"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -3953,19 +4184,19 @@
     </row>
     <row r="11" spans="1:15" ht="20" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="61"/>
+      <c r="C11" s="69"/>
       <c r="D11" s="44"/>
       <c r="E11" s="44"/>
       <c r="F11" s="44"/>
       <c r="G11" s="44"/>
       <c r="H11" s="44"/>
       <c r="I11" s="44"/>
-      <c r="J11" s="57"/>
-      <c r="K11" s="57"/>
-      <c r="L11" s="57"/>
+      <c r="J11" s="65"/>
+      <c r="K11" s="65"/>
+      <c r="L11" s="65"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
@@ -3994,11 +4225,11 @@
       <c r="I12" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="J12" s="58" t="s">
+      <c r="J12" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="K12" s="58"/>
-      <c r="L12" s="58"/>
+      <c r="K12" s="66"/>
+      <c r="L12" s="66"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
@@ -4027,11 +4258,11 @@
       <c r="I13" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="J13" s="52" t="s">
+      <c r="J13" s="60" t="s">
         <v>49</v>
       </c>
-      <c r="K13" s="52"/>
-      <c r="L13" s="52"/>
+      <c r="K13" s="60"/>
+      <c r="L13" s="60"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
@@ -4060,11 +4291,11 @@
       <c r="I14" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="J14" s="52" t="s">
+      <c r="J14" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="K14" s="52"/>
-      <c r="L14" s="52"/>
+      <c r="K14" s="60"/>
+      <c r="L14" s="60"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
@@ -4093,11 +4324,11 @@
       <c r="I15" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="J15" s="52" t="s">
+      <c r="J15" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="K15" s="52"/>
-      <c r="L15" s="52"/>
+      <c r="K15" s="60"/>
+      <c r="L15" s="60"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
@@ -4124,11 +4355,11 @@
       <c r="I16" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="J16" s="52" t="s">
+      <c r="J16" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="K16" s="52"/>
-      <c r="L16" s="52"/>
+      <c r="K16" s="60"/>
+      <c r="L16" s="60"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
@@ -4152,11 +4383,11 @@
     </row>
     <row r="18" spans="1:15" s="19" customFormat="1" ht="20" customHeight="1">
       <c r="A18" s="11"/>
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="59"/>
-      <c r="D18" s="59"/>
+      <c r="C18" s="67"/>
+      <c r="D18" s="67"/>
       <c r="E18" s="17"/>
       <c r="F18" s="18"/>
       <c r="G18" s="17"/>
@@ -4171,12 +4402,12 @@
     </row>
     <row r="19" spans="1:15" s="23" customFormat="1" ht="20" customHeight="1">
       <c r="A19" s="21"/>
-      <c r="B19" s="53" t="s">
+      <c r="B19" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="54"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="55"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="63"/>
       <c r="F19" s="50" t="s">
         <v>21</v>
       </c>
@@ -4365,10 +4596,10 @@
       <c r="A25" s="1"/>
       <c r="B25" s="31"/>
       <c r="C25" s="32"/>
-      <c r="D25" s="62" t="s">
+      <c r="D25" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="E25" s="63"/>
+      <c r="E25" s="56"/>
       <c r="F25" s="14" t="s">
         <v>59</v>
       </c>
@@ -4532,11 +4763,11 @@
     </row>
     <row r="34" spans="1:15" ht="20" customHeight="1">
       <c r="A34" s="1"/>
-      <c r="B34" s="56" t="s">
+      <c r="B34" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="C34" s="56"/>
-      <c r="D34" s="56"/>
+      <c r="C34" s="64"/>
+      <c r="D34" s="64"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
@@ -4551,12 +4782,12 @@
     </row>
     <row r="35" spans="1:15" ht="20" customHeight="1">
       <c r="A35" s="1"/>
-      <c r="B35" s="53" t="s">
+      <c r="B35" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="C35" s="54"/>
-      <c r="D35" s="54"/>
-      <c r="E35" s="55"/>
+      <c r="C35" s="62"/>
+      <c r="D35" s="62"/>
+      <c r="E35" s="63"/>
       <c r="F35" s="50" t="s">
         <v>21</v>
       </c>
@@ -4760,11 +4991,11 @@
     </row>
     <row r="42" spans="1:15" ht="20" customHeight="1">
       <c r="A42" s="1"/>
-      <c r="B42" s="56" t="s">
+      <c r="B42" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="56"/>
-      <c r="D42" s="56"/>
+      <c r="C42" s="64"/>
+      <c r="D42" s="64"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
@@ -4782,10 +5013,10 @@
       <c r="B43" s="49">
         <v>200</v>
       </c>
-      <c r="C43" s="62" t="s">
+      <c r="C43" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="D43" s="63"/>
+      <c r="D43" s="56"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
@@ -4803,10 +5034,10 @@
       <c r="B44" s="49">
         <v>401</v>
       </c>
-      <c r="C44" s="62" t="s">
+      <c r="C44" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="D44" s="63"/>
+      <c r="D44" s="56"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
@@ -4824,10 +5055,10 @@
       <c r="B45" s="49">
         <v>402</v>
       </c>
-      <c r="C45" s="62" t="s">
+      <c r="C45" s="55" t="s">
         <v>78</v>
       </c>
-      <c r="D45" s="63"/>
+      <c r="D45" s="56"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
@@ -4845,10 +5076,10 @@
       <c r="B46" s="49">
         <v>403</v>
       </c>
-      <c r="C46" s="62" t="s">
+      <c r="C46" s="55" t="s">
         <v>79</v>
       </c>
-      <c r="D46" s="63"/>
+      <c r="D46" s="56"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
@@ -4866,10 +5097,10 @@
       <c r="B47" s="39">
         <v>500</v>
       </c>
-      <c r="C47" s="64" t="s">
+      <c r="C47" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="D47" s="65"/>
+      <c r="D47" s="58"/>
       <c r="E47" s="34"/>
       <c r="F47" s="34"/>
       <c r="G47" s="34"/>
@@ -5785,10 +6016,2078 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="C5:I5"/>
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="C7:I7"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="J16:L16"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:E19"/>
     <mergeCell ref="C47:D47"/>
     <mergeCell ref="J14:L14"/>
     <mergeCell ref="J15:L15"/>
     <mergeCell ref="C46:D46"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="D25:E25"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="I13" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O99"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A27" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="12.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="2"/>
+    <col min="8" max="8" width="11.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.5" style="2" customWidth="1"/>
+    <col min="11" max="11" width="5.83203125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="38.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="20" customHeight="1">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+    </row>
+    <row r="2" spans="1:15" ht="20" customHeight="1">
+      <c r="A2" s="51" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+    </row>
+    <row r="3" spans="1:15" ht="20" customHeight="1">
+      <c r="A3" s="1"/>
+      <c r="B3" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+    </row>
+    <row r="4" spans="1:15" ht="20" customHeight="1">
+      <c r="A4" s="1"/>
+      <c r="B4" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="55" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+    </row>
+    <row r="5" spans="1:15" ht="20" customHeight="1">
+      <c r="A5" s="1"/>
+      <c r="B5" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="55" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="56"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+    </row>
+    <row r="6" spans="1:15" ht="20" customHeight="1">
+      <c r="A6" s="1"/>
+      <c r="B6" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="55" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="59"/>
+      <c r="G6" s="59"/>
+      <c r="H6" s="59"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+    </row>
+    <row r="7" spans="1:15" ht="20" customHeight="1">
+      <c r="A7" s="1"/>
+      <c r="B7" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="55" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="59"/>
+      <c r="G7" s="59"/>
+      <c r="H7" s="59"/>
+      <c r="I7" s="56"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+    </row>
+    <row r="8" spans="1:15" ht="20" customHeight="1">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="1:15" ht="20" customHeight="1">
+      <c r="A9" s="1"/>
+      <c r="B9" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="12"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+    </row>
+    <row r="10" spans="1:15" ht="20" customHeight="1">
+      <c r="A10" s="1"/>
+      <c r="B10" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="12"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+    </row>
+    <row r="11" spans="1:15" ht="20" customHeight="1">
+      <c r="A11" s="1"/>
+      <c r="B11" s="68" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="69"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="65"/>
+      <c r="K11" s="65"/>
+      <c r="L11" s="65"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+    </row>
+    <row r="12" spans="1:15" ht="20" customHeight="1">
+      <c r="A12" s="1"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="53" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="53" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="53" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="53" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="53" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12" s="66" t="s">
+        <v>20</v>
+      </c>
+      <c r="K12" s="66"/>
+      <c r="L12" s="66"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+    </row>
+    <row r="13" spans="1:15" ht="20" customHeight="1">
+      <c r="A13" s="1"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13" s="5">
+        <v>254</v>
+      </c>
+      <c r="I13" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="J13" s="60" t="s">
+        <v>49</v>
+      </c>
+      <c r="K13" s="60"/>
+      <c r="L13" s="60"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+    </row>
+    <row r="14" spans="1:15" ht="20" customHeight="1">
+      <c r="A14" s="1"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5">
+        <v>254</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="J14" s="60" t="s">
+        <v>44</v>
+      </c>
+      <c r="K14" s="60"/>
+      <c r="L14" s="60"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+    </row>
+    <row r="15" spans="1:15" ht="20" customHeight="1">
+      <c r="A15" s="1"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5">
+        <v>254</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="J15" s="60" t="s">
+        <v>44</v>
+      </c>
+      <c r="K15" s="60"/>
+      <c r="L15" s="60"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+    </row>
+    <row r="16" spans="1:15" ht="20" customHeight="1">
+      <c r="A16" s="1"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H16" s="5">
+        <v>254</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J16" s="60" t="s">
+        <v>44</v>
+      </c>
+      <c r="K16" s="60"/>
+      <c r="L16" s="60"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+    </row>
+    <row r="17" spans="1:15" ht="20" customHeight="1">
+      <c r="A17" s="1"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+    </row>
+    <row r="18" spans="1:15" s="19" customFormat="1" ht="20" customHeight="1">
+      <c r="A18" s="11"/>
+      <c r="B18" s="70" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="70"/>
+      <c r="D18" s="70"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
+    </row>
+    <row r="19" spans="1:15" s="23" customFormat="1" ht="20" customHeight="1">
+      <c r="A19" s="21"/>
+      <c r="B19" s="61" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="62"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="63"/>
+      <c r="F19" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" s="53" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="J19" s="53" t="s">
+        <v>17</v>
+      </c>
+      <c r="K19" s="53" t="s">
+        <v>18</v>
+      </c>
+      <c r="L19" s="53" t="s">
+        <v>20</v>
+      </c>
+      <c r="M19" s="21"/>
+      <c r="N19" s="21"/>
+      <c r="O19" s="21"/>
+    </row>
+    <row r="20" spans="1:15" ht="20" customHeight="1">
+      <c r="A20" s="1"/>
+      <c r="B20" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="L20" s="3"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+    </row>
+    <row r="21" spans="1:15" ht="20" customHeight="1">
+      <c r="A21" s="1"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="26"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I21" s="5">
+        <v>1</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="L21" s="3"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+    </row>
+    <row r="22" spans="1:15" ht="20" customHeight="1">
+      <c r="A22" s="1"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" s="24"/>
+      <c r="F22" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I22" s="5">
+        <v>1</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="L22" s="28"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+    </row>
+    <row r="23" spans="1:15" ht="20" customHeight="1">
+      <c r="A23" s="1"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H23" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="I23" s="5">
+        <v>1</v>
+      </c>
+      <c r="J23" s="5">
+        <v>3</v>
+      </c>
+      <c r="K23" s="5">
+        <v>3</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+    </row>
+    <row r="24" spans="1:15" ht="20" customHeight="1">
+      <c r="A24" s="1"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H24" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="I24" s="5">
+        <v>1</v>
+      </c>
+      <c r="J24" s="5">
+        <v>0</v>
+      </c>
+      <c r="K24" s="5">
+        <v>0</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+    </row>
+    <row r="25" spans="1:15" ht="20" customHeight="1">
+      <c r="A25" s="1"/>
+      <c r="B25" s="31"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25" s="56"/>
+      <c r="F25" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H25" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="I25" s="5">
+        <v>1</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K25" s="5">
+        <v>254</v>
+      </c>
+      <c r="L25" s="3"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+    </row>
+    <row r="26" spans="1:15" ht="20" customHeight="1">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+    </row>
+    <row r="27" spans="1:15" ht="20" customHeight="1">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+    </row>
+    <row r="28" spans="1:15" ht="20" customHeight="1">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+    </row>
+    <row r="29" spans="1:15" ht="20" customHeight="1">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+    </row>
+    <row r="30" spans="1:15" ht="20" customHeight="1">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+    </row>
+    <row r="31" spans="1:15" ht="20" customHeight="1">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+    </row>
+    <row r="32" spans="1:15" ht="20" customHeight="1">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+    </row>
+    <row r="33" spans="1:15" ht="20" customHeight="1">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+    </row>
+    <row r="34" spans="1:15" ht="20" customHeight="1">
+      <c r="A34" s="1"/>
+      <c r="B34" s="70" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" s="70"/>
+      <c r="D34" s="70"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+    </row>
+    <row r="35" spans="1:15" ht="20" customHeight="1">
+      <c r="A35" s="1"/>
+      <c r="B35" s="61" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" s="62"/>
+      <c r="D35" s="62"/>
+      <c r="E35" s="63"/>
+      <c r="F35" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="G35" s="53" t="s">
+        <v>15</v>
+      </c>
+      <c r="H35" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="I35" s="53" t="s">
+        <v>24</v>
+      </c>
+      <c r="J35" s="53" t="s">
+        <v>17</v>
+      </c>
+      <c r="K35" s="53" t="s">
+        <v>18</v>
+      </c>
+      <c r="L35" s="53" t="s">
+        <v>20</v>
+      </c>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+    </row>
+    <row r="36" spans="1:15" ht="20" customHeight="1">
+      <c r="A36" s="1"/>
+      <c r="B36" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K36" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="L36" s="3"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+    </row>
+    <row r="37" spans="1:15" ht="20" customHeight="1">
+      <c r="A37" s="4"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="D37" s="26"/>
+      <c r="E37" s="24"/>
+      <c r="F37" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K37" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="L37" s="3"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+    </row>
+    <row r="38" spans="1:15" ht="20" customHeight="1">
+      <c r="A38" s="4"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="E38" s="24"/>
+      <c r="F38" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K38" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="L38" s="28"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+      <c r="O38" s="1"/>
+    </row>
+    <row r="39" spans="1:15" ht="20" customHeight="1">
+      <c r="A39" s="4"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="F39" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H39" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="I39" s="5">
+        <v>1</v>
+      </c>
+      <c r="J39" s="5">
+        <v>3</v>
+      </c>
+      <c r="K39" s="5">
+        <v>3</v>
+      </c>
+      <c r="L39" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="1"/>
+    </row>
+    <row r="40" spans="1:15" s="37" customFormat="1" ht="20" customHeight="1">
+      <c r="A40" s="4"/>
+      <c r="B40" s="31"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="32"/>
+      <c r="E40" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="F40" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H40" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="I40" s="5">
+        <v>1</v>
+      </c>
+      <c r="J40" s="5">
+        <v>0</v>
+      </c>
+      <c r="K40" s="5">
+        <v>254</v>
+      </c>
+      <c r="L40" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M40" s="4"/>
+      <c r="N40" s="4"/>
+      <c r="O40" s="4"/>
+    </row>
+    <row r="41" spans="1:15" ht="20" customHeight="1">
+      <c r="A41" s="4"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
+      <c r="O41" s="1"/>
+    </row>
+    <row r="42" spans="1:15" ht="20" customHeight="1">
+      <c r="A42" s="1"/>
+      <c r="B42" s="70" t="s">
+        <v>33</v>
+      </c>
+      <c r="C42" s="70"/>
+      <c r="D42" s="70"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
+      <c r="M42" s="1"/>
+      <c r="N42" s="1"/>
+      <c r="O42" s="1"/>
+    </row>
+    <row r="43" spans="1:15" ht="20" customHeight="1">
+      <c r="A43" s="1"/>
+      <c r="B43" s="52">
+        <v>200</v>
+      </c>
+      <c r="C43" s="55" t="s">
+        <v>34</v>
+      </c>
+      <c r="D43" s="56"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+      <c r="L43" s="1"/>
+      <c r="M43" s="1"/>
+      <c r="N43" s="1"/>
+      <c r="O43" s="1"/>
+    </row>
+    <row r="44" spans="1:15" ht="20" customHeight="1">
+      <c r="A44" s="1"/>
+      <c r="B44" s="52">
+        <v>401</v>
+      </c>
+      <c r="C44" s="55" t="s">
+        <v>67</v>
+      </c>
+      <c r="D44" s="56"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1"/>
+      <c r="L44" s="1"/>
+      <c r="M44" s="1"/>
+      <c r="N44" s="1"/>
+      <c r="O44" s="1"/>
+    </row>
+    <row r="45" spans="1:15" ht="20" customHeight="1">
+      <c r="A45" s="1"/>
+      <c r="B45" s="52">
+        <v>402</v>
+      </c>
+      <c r="C45" s="55" t="s">
+        <v>68</v>
+      </c>
+      <c r="D45" s="56"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
+      <c r="L45" s="1"/>
+      <c r="M45" s="1"/>
+      <c r="N45" s="1"/>
+      <c r="O45" s="1"/>
+    </row>
+    <row r="46" spans="1:15" s="35" customFormat="1" ht="20" customHeight="1">
+      <c r="A46" s="34"/>
+      <c r="B46" s="39">
+        <v>500</v>
+      </c>
+      <c r="C46" s="57" t="s">
+        <v>38</v>
+      </c>
+      <c r="D46" s="58"/>
+      <c r="E46" s="34"/>
+      <c r="F46" s="34"/>
+      <c r="G46" s="34"/>
+      <c r="H46" s="34"/>
+      <c r="I46" s="34"/>
+      <c r="J46" s="34"/>
+      <c r="K46" s="34"/>
+      <c r="L46" s="34"/>
+      <c r="M46" s="34"/>
+      <c r="N46" s="34"/>
+      <c r="O46" s="34"/>
+    </row>
+    <row r="47" spans="1:15" ht="20" customHeight="1">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+      <c r="L47" s="1"/>
+      <c r="M47" s="1"/>
+      <c r="N47" s="1"/>
+      <c r="O47" s="1"/>
+    </row>
+    <row r="48" spans="1:15" s="35" customFormat="1" ht="20" customHeight="1">
+      <c r="A48" s="34"/>
+      <c r="B48" s="34"/>
+      <c r="C48" s="34"/>
+      <c r="D48" s="34"/>
+      <c r="E48" s="34"/>
+      <c r="F48" s="34"/>
+      <c r="G48" s="34"/>
+      <c r="H48" s="34"/>
+      <c r="I48" s="34"/>
+      <c r="J48" s="34"/>
+      <c r="K48" s="34"/>
+      <c r="L48" s="34"/>
+      <c r="M48" s="34"/>
+      <c r="N48" s="34"/>
+      <c r="O48" s="34"/>
+    </row>
+    <row r="49" spans="1:15" ht="20" customHeight="1">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
+      <c r="L49" s="1"/>
+      <c r="M49" s="1"/>
+      <c r="N49" s="1"/>
+      <c r="O49" s="1"/>
+    </row>
+    <row r="50" spans="1:15" s="35" customFormat="1" ht="20" customHeight="1">
+      <c r="A50" s="34"/>
+      <c r="B50" s="34"/>
+      <c r="C50" s="34"/>
+      <c r="D50" s="34"/>
+      <c r="E50" s="34"/>
+      <c r="F50" s="34"/>
+      <c r="G50" s="34"/>
+      <c r="H50" s="34"/>
+      <c r="I50" s="34"/>
+      <c r="J50" s="34"/>
+      <c r="K50" s="34"/>
+      <c r="L50" s="34"/>
+      <c r="M50" s="34"/>
+      <c r="N50" s="34"/>
+      <c r="O50" s="34"/>
+    </row>
+    <row r="51" spans="1:15" ht="20" customHeight="1">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
+      <c r="L51" s="1"/>
+      <c r="M51" s="1"/>
+      <c r="N51" s="1"/>
+      <c r="O51" s="1"/>
+    </row>
+    <row r="52" spans="1:15" ht="20" customHeight="1">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
+      <c r="L52" s="1"/>
+      <c r="M52" s="1"/>
+      <c r="N52" s="1"/>
+      <c r="O52" s="1"/>
+    </row>
+    <row r="53" spans="1:15" ht="20" customHeight="1">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
+      <c r="L53" s="1"/>
+      <c r="M53" s="1"/>
+      <c r="N53" s="1"/>
+      <c r="O53" s="1"/>
+    </row>
+    <row r="54" spans="1:15" ht="20" customHeight="1">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
+      <c r="L54" s="1"/>
+      <c r="M54" s="1"/>
+      <c r="N54" s="1"/>
+      <c r="O54" s="1"/>
+    </row>
+    <row r="55" spans="1:15" ht="20" customHeight="1">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+      <c r="K55" s="1"/>
+      <c r="L55" s="1"/>
+      <c r="M55" s="1"/>
+      <c r="N55" s="1"/>
+      <c r="O55" s="1"/>
+    </row>
+    <row r="56" spans="1:15" ht="20" customHeight="1">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
+      <c r="K56" s="1"/>
+      <c r="L56" s="1"/>
+      <c r="M56" s="1"/>
+      <c r="N56" s="1"/>
+      <c r="O56" s="1"/>
+    </row>
+    <row r="57" spans="1:15" ht="20" customHeight="1">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+      <c r="K57" s="1"/>
+      <c r="L57" s="1"/>
+      <c r="M57" s="1"/>
+      <c r="N57" s="1"/>
+      <c r="O57" s="1"/>
+    </row>
+    <row r="58" spans="1:15" ht="20" customHeight="1">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
+      <c r="K58" s="1"/>
+      <c r="L58" s="1"/>
+      <c r="M58" s="1"/>
+      <c r="N58" s="1"/>
+      <c r="O58" s="1"/>
+    </row>
+    <row r="59" spans="1:15" ht="20" customHeight="1">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1"/>
+      <c r="K59" s="1"/>
+      <c r="L59" s="1"/>
+      <c r="M59" s="1"/>
+      <c r="N59" s="1"/>
+      <c r="O59" s="1"/>
+    </row>
+    <row r="60" spans="1:15" ht="20" customHeight="1">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+      <c r="K60" s="1"/>
+      <c r="L60" s="1"/>
+      <c r="M60" s="1"/>
+      <c r="N60" s="1"/>
+      <c r="O60" s="1"/>
+    </row>
+    <row r="61" spans="1:15" ht="20" customHeight="1">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1"/>
+      <c r="K61" s="1"/>
+      <c r="L61" s="1"/>
+      <c r="M61" s="1"/>
+      <c r="N61" s="1"/>
+      <c r="O61" s="1"/>
+    </row>
+    <row r="62" spans="1:15" ht="20" customHeight="1">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+      <c r="J62" s="1"/>
+      <c r="K62" s="1"/>
+      <c r="L62" s="1"/>
+      <c r="M62" s="1"/>
+      <c r="N62" s="1"/>
+      <c r="O62" s="1"/>
+    </row>
+    <row r="63" spans="1:15" ht="20" customHeight="1">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
+      <c r="J63" s="1"/>
+      <c r="K63" s="1"/>
+      <c r="L63" s="1"/>
+      <c r="M63" s="1"/>
+      <c r="N63" s="1"/>
+      <c r="O63" s="1"/>
+    </row>
+    <row r="64" spans="1:15" ht="20" customHeight="1">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
+      <c r="H64" s="1"/>
+      <c r="I64" s="1"/>
+      <c r="J64" s="1"/>
+      <c r="K64" s="1"/>
+      <c r="L64" s="1"/>
+      <c r="M64" s="1"/>
+      <c r="N64" s="1"/>
+      <c r="O64" s="1"/>
+    </row>
+    <row r="65" spans="1:15" ht="20" customHeight="1">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+      <c r="J65" s="1"/>
+      <c r="K65" s="1"/>
+      <c r="L65" s="1"/>
+      <c r="M65" s="1"/>
+      <c r="N65" s="1"/>
+      <c r="O65" s="1"/>
+    </row>
+    <row r="66" spans="1:15" ht="20" customHeight="1">
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="1"/>
+      <c r="J66" s="1"/>
+      <c r="K66" s="1"/>
+      <c r="L66" s="1"/>
+      <c r="M66" s="1"/>
+      <c r="N66" s="1"/>
+      <c r="O66" s="1"/>
+    </row>
+    <row r="67" spans="1:15" ht="20" customHeight="1">
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
+      <c r="J67" s="1"/>
+      <c r="K67" s="1"/>
+      <c r="L67" s="1"/>
+      <c r="M67" s="1"/>
+      <c r="N67" s="1"/>
+      <c r="O67" s="1"/>
+    </row>
+    <row r="68" spans="1:15" ht="20" customHeight="1">
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+      <c r="I68" s="1"/>
+      <c r="J68" s="1"/>
+      <c r="K68" s="1"/>
+      <c r="L68" s="1"/>
+      <c r="M68" s="1"/>
+      <c r="N68" s="1"/>
+      <c r="O68" s="1"/>
+    </row>
+    <row r="69" spans="1:15" ht="20" customHeight="1">
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
+      <c r="I69" s="1"/>
+      <c r="J69" s="1"/>
+      <c r="K69" s="1"/>
+      <c r="L69" s="1"/>
+      <c r="M69" s="1"/>
+      <c r="N69" s="1"/>
+      <c r="O69" s="1"/>
+    </row>
+    <row r="70" spans="1:15" ht="20" customHeight="1">
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
+      <c r="J70" s="1"/>
+      <c r="K70" s="1"/>
+      <c r="L70" s="1"/>
+      <c r="M70" s="1"/>
+      <c r="N70" s="1"/>
+      <c r="O70" s="1"/>
+    </row>
+    <row r="71" spans="1:15" ht="20" customHeight="1">
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+      <c r="G71" s="1"/>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1"/>
+      <c r="J71" s="1"/>
+      <c r="K71" s="1"/>
+      <c r="L71" s="1"/>
+      <c r="M71" s="1"/>
+      <c r="N71" s="1"/>
+      <c r="O71" s="1"/>
+    </row>
+    <row r="72" spans="1:15" ht="20" customHeight="1">
+      <c r="A72" s="1"/>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
+      <c r="H72" s="1"/>
+      <c r="I72" s="1"/>
+      <c r="J72" s="1"/>
+      <c r="K72" s="1"/>
+      <c r="L72" s="1"/>
+      <c r="M72" s="1"/>
+      <c r="N72" s="1"/>
+      <c r="O72" s="1"/>
+    </row>
+    <row r="73" spans="1:15" ht="20" customHeight="1">
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+      <c r="H73" s="1"/>
+      <c r="I73" s="1"/>
+      <c r="J73" s="1"/>
+      <c r="K73" s="1"/>
+      <c r="L73" s="1"/>
+      <c r="M73" s="1"/>
+      <c r="N73" s="1"/>
+      <c r="O73" s="1"/>
+    </row>
+    <row r="74" spans="1:15" ht="20" customHeight="1">
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+      <c r="G74" s="1"/>
+      <c r="H74" s="1"/>
+      <c r="I74" s="1"/>
+      <c r="J74" s="1"/>
+      <c r="K74" s="1"/>
+      <c r="L74" s="1"/>
+      <c r="M74" s="1"/>
+      <c r="N74" s="1"/>
+      <c r="O74" s="1"/>
+    </row>
+    <row r="75" spans="1:15" ht="20" customHeight="1">
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
+      <c r="H75" s="1"/>
+      <c r="I75" s="1"/>
+      <c r="J75" s="1"/>
+      <c r="K75" s="1"/>
+      <c r="L75" s="1"/>
+      <c r="M75" s="1"/>
+      <c r="N75" s="1"/>
+      <c r="O75" s="1"/>
+    </row>
+    <row r="76" spans="1:15" ht="20" customHeight="1">
+      <c r="A76" s="1"/>
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+      <c r="G76" s="1"/>
+      <c r="H76" s="1"/>
+      <c r="I76" s="1"/>
+      <c r="J76" s="1"/>
+      <c r="K76" s="1"/>
+      <c r="L76" s="1"/>
+      <c r="M76" s="1"/>
+      <c r="N76" s="1"/>
+      <c r="O76" s="1"/>
+    </row>
+    <row r="77" spans="1:15" ht="20" customHeight="1">
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+      <c r="F77" s="1"/>
+      <c r="G77" s="1"/>
+      <c r="H77" s="1"/>
+      <c r="I77" s="1"/>
+      <c r="J77" s="1"/>
+      <c r="K77" s="1"/>
+      <c r="L77" s="1"/>
+      <c r="M77" s="1"/>
+      <c r="N77" s="1"/>
+      <c r="O77" s="1"/>
+    </row>
+    <row r="78" spans="1:15" ht="20" customHeight="1">
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
+      <c r="F78" s="1"/>
+      <c r="G78" s="1"/>
+      <c r="H78" s="1"/>
+      <c r="I78" s="1"/>
+      <c r="J78" s="1"/>
+      <c r="K78" s="1"/>
+      <c r="L78" s="1"/>
+      <c r="M78" s="1"/>
+      <c r="N78" s="1"/>
+      <c r="O78" s="1"/>
+    </row>
+    <row r="79" spans="1:15" ht="20" customHeight="1">
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1"/>
+      <c r="F79" s="1"/>
+      <c r="G79" s="1"/>
+      <c r="H79" s="1"/>
+      <c r="I79" s="1"/>
+      <c r="J79" s="1"/>
+      <c r="K79" s="1"/>
+      <c r="L79" s="1"/>
+      <c r="M79" s="1"/>
+      <c r="N79" s="1"/>
+      <c r="O79" s="1"/>
+    </row>
+    <row r="80" spans="1:15" ht="20" customHeight="1">
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
+      <c r="D80" s="1"/>
+      <c r="E80" s="1"/>
+      <c r="F80" s="1"/>
+      <c r="G80" s="1"/>
+      <c r="H80" s="1"/>
+      <c r="I80" s="1"/>
+      <c r="J80" s="1"/>
+      <c r="K80" s="1"/>
+      <c r="L80" s="1"/>
+      <c r="M80" s="1"/>
+      <c r="N80" s="1"/>
+      <c r="O80" s="1"/>
+    </row>
+    <row r="81" spans="1:15" ht="20" customHeight="1">
+      <c r="A81" s="1"/>
+      <c r="B81" s="1"/>
+      <c r="C81" s="1"/>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1"/>
+      <c r="F81" s="1"/>
+      <c r="G81" s="1"/>
+      <c r="H81" s="1"/>
+      <c r="I81" s="1"/>
+      <c r="J81" s="1"/>
+      <c r="K81" s="1"/>
+      <c r="L81" s="1"/>
+      <c r="M81" s="1"/>
+      <c r="N81" s="1"/>
+      <c r="O81" s="1"/>
+    </row>
+    <row r="82" spans="1:15" ht="20" customHeight="1">
+      <c r="A82" s="1"/>
+      <c r="B82" s="1"/>
+      <c r="C82" s="1"/>
+      <c r="D82" s="1"/>
+      <c r="E82" s="1"/>
+      <c r="F82" s="1"/>
+      <c r="G82" s="1"/>
+      <c r="H82" s="1"/>
+      <c r="I82" s="1"/>
+      <c r="J82" s="1"/>
+      <c r="K82" s="1"/>
+      <c r="L82" s="1"/>
+      <c r="M82" s="1"/>
+      <c r="N82" s="1"/>
+      <c r="O82" s="1"/>
+    </row>
+    <row r="83" spans="1:15" ht="20" customHeight="1">
+      <c r="A83" s="1"/>
+      <c r="B83" s="1"/>
+      <c r="C83" s="1"/>
+      <c r="D83" s="1"/>
+      <c r="E83" s="1"/>
+      <c r="F83" s="1"/>
+      <c r="G83" s="1"/>
+      <c r="H83" s="1"/>
+      <c r="I83" s="1"/>
+      <c r="J83" s="1"/>
+      <c r="K83" s="1"/>
+      <c r="L83" s="1"/>
+      <c r="M83" s="1"/>
+      <c r="N83" s="1"/>
+      <c r="O83" s="1"/>
+    </row>
+    <row r="84" spans="1:15" ht="20" customHeight="1">
+      <c r="A84" s="1"/>
+      <c r="B84" s="1"/>
+      <c r="C84" s="1"/>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1"/>
+      <c r="F84" s="1"/>
+      <c r="G84" s="1"/>
+      <c r="H84" s="1"/>
+      <c r="I84" s="1"/>
+      <c r="J84" s="1"/>
+      <c r="K84" s="1"/>
+      <c r="L84" s="1"/>
+      <c r="M84" s="1"/>
+      <c r="N84" s="1"/>
+      <c r="O84" s="1"/>
+    </row>
+    <row r="85" spans="1:15" ht="20" customHeight="1">
+      <c r="A85" s="1"/>
+      <c r="B85" s="1"/>
+      <c r="C85" s="1"/>
+      <c r="D85" s="1"/>
+      <c r="E85" s="1"/>
+      <c r="F85" s="1"/>
+      <c r="G85" s="1"/>
+      <c r="H85" s="1"/>
+      <c r="I85" s="1"/>
+      <c r="J85" s="1"/>
+      <c r="K85" s="1"/>
+      <c r="L85" s="1"/>
+      <c r="M85" s="1"/>
+      <c r="N85" s="1"/>
+      <c r="O85" s="1"/>
+    </row>
+    <row r="86" spans="1:15" ht="20" customHeight="1">
+      <c r="A86" s="1"/>
+      <c r="B86" s="1"/>
+      <c r="C86" s="1"/>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1"/>
+      <c r="F86" s="1"/>
+      <c r="G86" s="1"/>
+      <c r="H86" s="1"/>
+      <c r="I86" s="1"/>
+      <c r="J86" s="1"/>
+      <c r="K86" s="1"/>
+      <c r="L86" s="1"/>
+      <c r="M86" s="1"/>
+      <c r="N86" s="1"/>
+      <c r="O86" s="1"/>
+    </row>
+    <row r="87" spans="1:15" ht="20" customHeight="1">
+      <c r="A87" s="1"/>
+      <c r="B87" s="1"/>
+      <c r="C87" s="1"/>
+      <c r="D87" s="1"/>
+      <c r="E87" s="1"/>
+      <c r="F87" s="1"/>
+      <c r="G87" s="1"/>
+      <c r="H87" s="1"/>
+      <c r="I87" s="1"/>
+      <c r="J87" s="1"/>
+      <c r="K87" s="1"/>
+      <c r="L87" s="1"/>
+      <c r="M87" s="1"/>
+      <c r="N87" s="1"/>
+      <c r="O87" s="1"/>
+    </row>
+    <row r="88" spans="1:15" ht="20" customHeight="1">
+      <c r="A88" s="1"/>
+      <c r="B88" s="1"/>
+      <c r="C88" s="1"/>
+      <c r="D88" s="1"/>
+      <c r="E88" s="1"/>
+      <c r="F88" s="1"/>
+      <c r="G88" s="1"/>
+      <c r="H88" s="1"/>
+      <c r="I88" s="1"/>
+      <c r="J88" s="1"/>
+      <c r="K88" s="1"/>
+      <c r="L88" s="1"/>
+      <c r="M88" s="1"/>
+      <c r="N88" s="1"/>
+      <c r="O88" s="1"/>
+    </row>
+    <row r="89" spans="1:15" ht="20" customHeight="1">
+      <c r="A89" s="1"/>
+      <c r="B89" s="1"/>
+      <c r="C89" s="1"/>
+      <c r="D89" s="1"/>
+      <c r="E89" s="1"/>
+      <c r="F89" s="1"/>
+      <c r="G89" s="1"/>
+      <c r="H89" s="1"/>
+      <c r="I89" s="1"/>
+      <c r="J89" s="1"/>
+      <c r="K89" s="1"/>
+      <c r="L89" s="1"/>
+      <c r="M89" s="1"/>
+      <c r="N89" s="1"/>
+      <c r="O89" s="1"/>
+    </row>
+    <row r="90" spans="1:15" ht="20" customHeight="1">
+      <c r="A90" s="1"/>
+      <c r="B90" s="1"/>
+      <c r="C90" s="1"/>
+      <c r="D90" s="1"/>
+      <c r="E90" s="1"/>
+      <c r="F90" s="1"/>
+      <c r="G90" s="1"/>
+      <c r="H90" s="1"/>
+      <c r="I90" s="1"/>
+      <c r="J90" s="1"/>
+      <c r="K90" s="1"/>
+      <c r="L90" s="1"/>
+      <c r="M90" s="1"/>
+      <c r="N90" s="1"/>
+      <c r="O90" s="1"/>
+    </row>
+    <row r="91" spans="1:15" ht="20" customHeight="1">
+      <c r="A91" s="1"/>
+      <c r="B91" s="1"/>
+      <c r="C91" s="1"/>
+      <c r="D91" s="1"/>
+      <c r="E91" s="1"/>
+      <c r="F91" s="1"/>
+      <c r="G91" s="1"/>
+      <c r="H91" s="1"/>
+      <c r="I91" s="1"/>
+      <c r="J91" s="1"/>
+      <c r="K91" s="1"/>
+      <c r="L91" s="1"/>
+      <c r="M91" s="1"/>
+      <c r="N91" s="1"/>
+      <c r="O91" s="1"/>
+    </row>
+    <row r="92" spans="1:15" ht="20" customHeight="1">
+      <c r="A92" s="1"/>
+      <c r="B92" s="1"/>
+      <c r="C92" s="1"/>
+      <c r="D92" s="1"/>
+      <c r="E92" s="1"/>
+      <c r="F92" s="1"/>
+      <c r="G92" s="1"/>
+      <c r="H92" s="1"/>
+      <c r="I92" s="1"/>
+      <c r="J92" s="1"/>
+      <c r="K92" s="1"/>
+      <c r="L92" s="1"/>
+      <c r="M92" s="1"/>
+      <c r="N92" s="1"/>
+      <c r="O92" s="1"/>
+    </row>
+    <row r="93" spans="1:15" ht="20" customHeight="1">
+      <c r="A93" s="1"/>
+      <c r="B93" s="1"/>
+      <c r="C93" s="1"/>
+      <c r="D93" s="1"/>
+      <c r="E93" s="1"/>
+      <c r="F93" s="1"/>
+      <c r="G93" s="1"/>
+      <c r="H93" s="1"/>
+      <c r="I93" s="1"/>
+      <c r="J93" s="1"/>
+      <c r="K93" s="1"/>
+      <c r="L93" s="1"/>
+      <c r="M93" s="1"/>
+      <c r="N93" s="1"/>
+      <c r="O93" s="1"/>
+    </row>
+    <row r="94" spans="1:15" ht="20" customHeight="1">
+      <c r="A94" s="1"/>
+      <c r="B94" s="1"/>
+      <c r="C94" s="1"/>
+      <c r="D94" s="1"/>
+      <c r="E94" s="1"/>
+      <c r="F94" s="1"/>
+      <c r="G94" s="1"/>
+      <c r="H94" s="1"/>
+      <c r="I94" s="1"/>
+      <c r="J94" s="1"/>
+      <c r="K94" s="1"/>
+      <c r="L94" s="1"/>
+      <c r="M94" s="1"/>
+      <c r="N94" s="1"/>
+      <c r="O94" s="1"/>
+    </row>
+    <row r="95" spans="1:15" ht="20" customHeight="1">
+      <c r="A95" s="1"/>
+      <c r="B95" s="1"/>
+      <c r="C95" s="1"/>
+      <c r="D95" s="1"/>
+      <c r="E95" s="1"/>
+      <c r="F95" s="1"/>
+      <c r="G95" s="1"/>
+      <c r="H95" s="1"/>
+      <c r="I95" s="1"/>
+      <c r="J95" s="1"/>
+      <c r="K95" s="1"/>
+      <c r="L95" s="1"/>
+      <c r="M95" s="1"/>
+      <c r="N95" s="1"/>
+      <c r="O95" s="1"/>
+    </row>
+    <row r="96" spans="1:15" ht="20" customHeight="1">
+      <c r="A96" s="1"/>
+      <c r="B96" s="1"/>
+      <c r="C96" s="1"/>
+      <c r="D96" s="1"/>
+      <c r="E96" s="1"/>
+      <c r="F96" s="1"/>
+      <c r="G96" s="1"/>
+      <c r="H96" s="1"/>
+      <c r="I96" s="1"/>
+      <c r="J96" s="1"/>
+      <c r="K96" s="1"/>
+      <c r="L96" s="1"/>
+      <c r="M96" s="1"/>
+      <c r="N96" s="1"/>
+      <c r="O96" s="1"/>
+    </row>
+    <row r="97" spans="1:15" ht="20" customHeight="1">
+      <c r="A97" s="1"/>
+      <c r="B97" s="1"/>
+      <c r="C97" s="1"/>
+      <c r="D97" s="1"/>
+      <c r="E97" s="1"/>
+      <c r="F97" s="1"/>
+      <c r="G97" s="1"/>
+      <c r="H97" s="1"/>
+      <c r="I97" s="1"/>
+      <c r="J97" s="1"/>
+      <c r="K97" s="1"/>
+      <c r="L97" s="1"/>
+      <c r="M97" s="1"/>
+      <c r="N97" s="1"/>
+      <c r="O97" s="1"/>
+    </row>
+    <row r="98" spans="1:15" ht="20" customHeight="1">
+      <c r="A98" s="1"/>
+      <c r="B98" s="1"/>
+      <c r="C98" s="1"/>
+      <c r="D98" s="1"/>
+      <c r="E98" s="1"/>
+      <c r="F98" s="1"/>
+      <c r="G98" s="1"/>
+      <c r="H98" s="1"/>
+      <c r="I98" s="1"/>
+      <c r="J98" s="1"/>
+      <c r="K98" s="1"/>
+      <c r="L98" s="1"/>
+      <c r="M98" s="1"/>
+      <c r="N98" s="1"/>
+      <c r="O98" s="1"/>
+    </row>
+    <row r="99" spans="1:15" ht="20" customHeight="1">
+      <c r="A99" s="36"/>
+      <c r="B99" s="36"/>
+      <c r="C99" s="36"/>
+      <c r="D99" s="36"/>
+      <c r="E99" s="36"/>
+      <c r="F99" s="36"/>
+      <c r="G99" s="36"/>
+      <c r="H99" s="36"/>
+      <c r="I99" s="36"/>
+      <c r="J99" s="36"/>
+      <c r="K99" s="36"/>
+      <c r="L99" s="36"/>
+      <c r="M99" s="36"/>
+      <c r="N99" s="36"/>
+      <c r="O99" s="36"/>
+    </row>
+  </sheetData>
+  <mergeCells count="21">
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="J14:L14"/>
     <mergeCell ref="B34:D34"/>
     <mergeCell ref="B35:E35"/>
     <mergeCell ref="B42:D42"/>

</xml_diff>

<commit_message>
finish 3 docs for post/comment
</commit_message>
<xml_diff>
--- a/spec/PHP_Training_Task17060_APIFormat_Ver_0.1.0.xlsx
+++ b/spec/PHP_Training_Task17060_APIFormat_Ver_0.1.0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7280" yWindow="860" windowWidth="25600" windowHeight="15540" tabRatio="640" activeTab="3"/>
+    <workbookView xWindow="6860" yWindow="2040" windowWidth="25600" windowHeight="15540" tabRatio="640" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="API List" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="115">
   <si>
     <t>No</t>
   </si>
@@ -367,9 +367,6 @@
     <t>Text</t>
   </si>
   <si>
-    <t>The API is used when user want to up a post and comment.</t>
-  </si>
-  <si>
     <t>a post or comment content</t>
   </si>
   <si>
@@ -395,6 +392,12 @@
   </si>
   <si>
     <t>Updatepassword</t>
+  </si>
+  <si>
+    <t>repassword</t>
+  </si>
+  <si>
+    <t>The API is used when user want to up a post or comment.</t>
   </si>
 </sst>
 </file>
@@ -661,7 +664,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="81">
+  <cellStyleXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -700,6 +703,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -849,6 +855,13 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="37" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -897,15 +910,8 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="37" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="81">
+  <cellStyles count="84">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -967,6 +973,9 @@
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1343,13 +1352,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>540026</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>167311</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>629477</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>110435</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2134,7 +2143,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="53" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>88</v>
@@ -2151,7 +2160,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="53" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>90</v>
@@ -2394,15 +2403,15 @@
       <c r="B4" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="58" t="s">
+      <c r="C4" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="62"/>
-      <c r="I4" s="59"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="64"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
@@ -2415,15 +2424,15 @@
       <c r="B5" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="58" t="s">
+      <c r="C5" s="63" t="s">
         <v>63</v>
       </c>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
-      <c r="H5" s="62"/>
-      <c r="I5" s="59"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="64"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -2436,15 +2445,15 @@
       <c r="B6" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="58" t="s">
+      <c r="C6" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="62"/>
-      <c r="E6" s="62"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="62"/>
-      <c r="H6" s="62"/>
-      <c r="I6" s="59"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="67"/>
+      <c r="H6" s="67"/>
+      <c r="I6" s="64"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -2457,15 +2466,15 @@
       <c r="B7" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="58" t="s">
+      <c r="C7" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="62"/>
-      <c r="H7" s="62"/>
-      <c r="I7" s="59"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="67"/>
+      <c r="I7" s="64"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -2530,19 +2539,19 @@
     </row>
     <row r="11" spans="1:15" ht="20" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="71" t="s">
+      <c r="B11" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="72"/>
+      <c r="C11" s="77"/>
       <c r="D11" s="44"/>
       <c r="E11" s="44"/>
       <c r="F11" s="44"/>
       <c r="G11" s="44"/>
       <c r="H11" s="44"/>
       <c r="I11" s="44"/>
-      <c r="J11" s="68"/>
-      <c r="K11" s="68"/>
-      <c r="L11" s="68"/>
+      <c r="J11" s="73"/>
+      <c r="K11" s="73"/>
+      <c r="L11" s="73"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
@@ -2571,11 +2580,11 @@
       <c r="I12" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="J12" s="69" t="s">
+      <c r="J12" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="K12" s="69"/>
-      <c r="L12" s="69"/>
+      <c r="K12" s="74"/>
+      <c r="L12" s="74"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
@@ -2604,11 +2613,11 @@
       <c r="I13" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="J13" s="63" t="s">
+      <c r="J13" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="K13" s="63"/>
-      <c r="L13" s="63"/>
+      <c r="K13" s="68"/>
+      <c r="L13" s="68"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
@@ -2637,11 +2646,11 @@
       <c r="I14" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="J14" s="63" t="s">
+      <c r="J14" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="K14" s="63"/>
-      <c r="L14" s="63"/>
+      <c r="K14" s="68"/>
+      <c r="L14" s="68"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
@@ -2665,11 +2674,11 @@
     </row>
     <row r="16" spans="1:15" s="19" customFormat="1" ht="20" customHeight="1">
       <c r="A16" s="11"/>
-      <c r="B16" s="70" t="s">
+      <c r="B16" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="70"/>
-      <c r="D16" s="70"/>
+      <c r="C16" s="75"/>
+      <c r="D16" s="75"/>
       <c r="E16" s="17"/>
       <c r="F16" s="18"/>
       <c r="G16" s="17"/>
@@ -2684,12 +2693,12 @@
     </row>
     <row r="17" spans="1:15" s="23" customFormat="1" ht="20" customHeight="1">
       <c r="A17" s="21"/>
-      <c r="B17" s="64" t="s">
+      <c r="B17" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="65"/>
-      <c r="D17" s="65"/>
-      <c r="E17" s="66"/>
+      <c r="C17" s="70"/>
+      <c r="D17" s="70"/>
+      <c r="E17" s="71"/>
       <c r="F17" s="22" t="s">
         <v>21</v>
       </c>
@@ -2878,10 +2887,10 @@
       <c r="A23" s="1"/>
       <c r="B23" s="31"/>
       <c r="C23" s="32"/>
-      <c r="D23" s="58" t="s">
+      <c r="D23" s="63" t="s">
         <v>58</v>
       </c>
-      <c r="E23" s="59"/>
+      <c r="E23" s="64"/>
       <c r="F23" s="14" t="s">
         <v>59</v>
       </c>
@@ -3045,11 +3054,11 @@
     </row>
     <row r="32" spans="1:15" ht="20" customHeight="1">
       <c r="A32" s="1"/>
-      <c r="B32" s="67" t="s">
+      <c r="B32" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="67"/>
-      <c r="D32" s="67"/>
+      <c r="C32" s="72"/>
+      <c r="D32" s="72"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
@@ -3064,12 +3073,12 @@
     </row>
     <row r="33" spans="1:15" ht="20" customHeight="1">
       <c r="A33" s="1"/>
-      <c r="B33" s="64" t="s">
+      <c r="B33" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="C33" s="65"/>
-      <c r="D33" s="65"/>
-      <c r="E33" s="66"/>
+      <c r="C33" s="70"/>
+      <c r="D33" s="70"/>
+      <c r="E33" s="71"/>
       <c r="F33" s="22" t="s">
         <v>21</v>
       </c>
@@ -3273,11 +3282,11 @@
     </row>
     <row r="40" spans="1:15" ht="20" customHeight="1">
       <c r="A40" s="1"/>
-      <c r="B40" s="67" t="s">
+      <c r="B40" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="C40" s="67"/>
-      <c r="D40" s="67"/>
+      <c r="C40" s="72"/>
+      <c r="D40" s="72"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
@@ -3295,10 +3304,10 @@
       <c r="B41" s="38">
         <v>200</v>
       </c>
-      <c r="C41" s="58" t="s">
+      <c r="C41" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="D41" s="59"/>
+      <c r="D41" s="64"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
@@ -3316,10 +3325,10 @@
       <c r="B42" s="38">
         <v>401</v>
       </c>
-      <c r="C42" s="58" t="s">
+      <c r="C42" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="D42" s="59"/>
+      <c r="D42" s="64"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
@@ -3337,10 +3346,10 @@
       <c r="B43" s="45">
         <v>402</v>
       </c>
-      <c r="C43" s="58" t="s">
+      <c r="C43" s="63" t="s">
         <v>68</v>
       </c>
-      <c r="D43" s="59"/>
+      <c r="D43" s="64"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
@@ -3358,10 +3367,10 @@
       <c r="B44" s="39">
         <v>500</v>
       </c>
-      <c r="C44" s="60" t="s">
+      <c r="C44" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="D44" s="61"/>
+      <c r="D44" s="66"/>
       <c r="E44" s="34"/>
       <c r="F44" s="34"/>
       <c r="G44" s="34"/>
@@ -4399,15 +4408,15 @@
       <c r="B4" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="58" t="s">
+      <c r="C4" s="63" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="62"/>
-      <c r="I4" s="59"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="64"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
@@ -4420,15 +4429,15 @@
       <c r="B5" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="58" t="s">
+      <c r="C5" s="63" t="s">
         <v>70</v>
       </c>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
-      <c r="H5" s="62"/>
-      <c r="I5" s="59"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="64"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -4441,15 +4450,15 @@
       <c r="B6" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="58" t="s">
+      <c r="C6" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="62"/>
-      <c r="E6" s="62"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="62"/>
-      <c r="H6" s="62"/>
-      <c r="I6" s="59"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="67"/>
+      <c r="H6" s="67"/>
+      <c r="I6" s="64"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -4462,15 +4471,15 @@
       <c r="B7" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="58" t="s">
+      <c r="C7" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="62"/>
-      <c r="H7" s="62"/>
-      <c r="I7" s="59"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="67"/>
+      <c r="I7" s="64"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -4535,19 +4544,19 @@
     </row>
     <row r="11" spans="1:15" ht="20" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="71" t="s">
+      <c r="B11" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="72"/>
+      <c r="C11" s="77"/>
       <c r="D11" s="44"/>
       <c r="E11" s="44"/>
       <c r="F11" s="44"/>
       <c r="G11" s="44"/>
       <c r="H11" s="44"/>
       <c r="I11" s="44"/>
-      <c r="J11" s="68"/>
-      <c r="K11" s="68"/>
-      <c r="L11" s="68"/>
+      <c r="J11" s="73"/>
+      <c r="K11" s="73"/>
+      <c r="L11" s="73"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
@@ -4576,11 +4585,11 @@
       <c r="I12" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="J12" s="69" t="s">
+      <c r="J12" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="K12" s="69"/>
-      <c r="L12" s="69"/>
+      <c r="K12" s="74"/>
+      <c r="L12" s="74"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
@@ -4609,11 +4618,11 @@
       <c r="I13" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="J13" s="63" t="s">
+      <c r="J13" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="K13" s="63"/>
-      <c r="L13" s="63"/>
+      <c r="K13" s="68"/>
+      <c r="L13" s="68"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
@@ -4642,11 +4651,11 @@
       <c r="I14" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="J14" s="63" t="s">
+      <c r="J14" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="K14" s="63"/>
-      <c r="L14" s="63"/>
+      <c r="K14" s="68"/>
+      <c r="L14" s="68"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
@@ -4675,11 +4684,11 @@
       <c r="I15" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="J15" s="63" t="s">
+      <c r="J15" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="K15" s="63"/>
-      <c r="L15" s="63"/>
+      <c r="K15" s="68"/>
+      <c r="L15" s="68"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
@@ -4706,11 +4715,11 @@
       <c r="I16" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="J16" s="63" t="s">
+      <c r="J16" s="68" t="s">
         <v>77</v>
       </c>
-      <c r="K16" s="63"/>
-      <c r="L16" s="63"/>
+      <c r="K16" s="68"/>
+      <c r="L16" s="68"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
@@ -4734,11 +4743,11 @@
     </row>
     <row r="18" spans="1:15" s="19" customFormat="1" ht="20" customHeight="1">
       <c r="A18" s="11"/>
-      <c r="B18" s="70" t="s">
+      <c r="B18" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="70"/>
-      <c r="D18" s="70"/>
+      <c r="C18" s="75"/>
+      <c r="D18" s="75"/>
       <c r="E18" s="17"/>
       <c r="F18" s="18"/>
       <c r="G18" s="17"/>
@@ -4753,12 +4762,12 @@
     </row>
     <row r="19" spans="1:15" s="23" customFormat="1" ht="20" customHeight="1">
       <c r="A19" s="21"/>
-      <c r="B19" s="64" t="s">
+      <c r="B19" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="65"/>
-      <c r="D19" s="65"/>
-      <c r="E19" s="66"/>
+      <c r="C19" s="70"/>
+      <c r="D19" s="70"/>
+      <c r="E19" s="71"/>
       <c r="F19" s="50" t="s">
         <v>21</v>
       </c>
@@ -4947,10 +4956,10 @@
       <c r="A25" s="1"/>
       <c r="B25" s="31"/>
       <c r="C25" s="32"/>
-      <c r="D25" s="58" t="s">
+      <c r="D25" s="63" t="s">
         <v>58</v>
       </c>
-      <c r="E25" s="59"/>
+      <c r="E25" s="64"/>
       <c r="F25" s="14" t="s">
         <v>59</v>
       </c>
@@ -5114,11 +5123,11 @@
     </row>
     <row r="34" spans="1:15" ht="20" customHeight="1">
       <c r="A34" s="1"/>
-      <c r="B34" s="67" t="s">
+      <c r="B34" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="C34" s="67"/>
-      <c r="D34" s="67"/>
+      <c r="C34" s="72"/>
+      <c r="D34" s="72"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
@@ -5133,12 +5142,12 @@
     </row>
     <row r="35" spans="1:15" ht="20" customHeight="1">
       <c r="A35" s="1"/>
-      <c r="B35" s="64" t="s">
+      <c r="B35" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="C35" s="65"/>
-      <c r="D35" s="65"/>
-      <c r="E35" s="66"/>
+      <c r="C35" s="70"/>
+      <c r="D35" s="70"/>
+      <c r="E35" s="71"/>
       <c r="F35" s="50" t="s">
         <v>21</v>
       </c>
@@ -5342,11 +5351,11 @@
     </row>
     <row r="42" spans="1:15" ht="20" customHeight="1">
       <c r="A42" s="1"/>
-      <c r="B42" s="67" t="s">
+      <c r="B42" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="67"/>
-      <c r="D42" s="67"/>
+      <c r="C42" s="72"/>
+      <c r="D42" s="72"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
@@ -5364,10 +5373,10 @@
       <c r="B43" s="49">
         <v>200</v>
       </c>
-      <c r="C43" s="58" t="s">
+      <c r="C43" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="D43" s="59"/>
+      <c r="D43" s="64"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
@@ -5385,10 +5394,10 @@
       <c r="B44" s="49">
         <v>401</v>
       </c>
-      <c r="C44" s="58" t="s">
+      <c r="C44" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="D44" s="59"/>
+      <c r="D44" s="64"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
@@ -5406,10 +5415,10 @@
       <c r="B45" s="49">
         <v>402</v>
       </c>
-      <c r="C45" s="58" t="s">
+      <c r="C45" s="63" t="s">
         <v>78</v>
       </c>
-      <c r="D45" s="59"/>
+      <c r="D45" s="64"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
@@ -5427,10 +5436,10 @@
       <c r="B46" s="49">
         <v>403</v>
       </c>
-      <c r="C46" s="58" t="s">
+      <c r="C46" s="63" t="s">
         <v>79</v>
       </c>
-      <c r="D46" s="59"/>
+      <c r="D46" s="64"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
@@ -5448,10 +5457,10 @@
       <c r="B47" s="39">
         <v>500</v>
       </c>
-      <c r="C47" s="60" t="s">
+      <c r="C47" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="D47" s="61"/>
+      <c r="D47" s="66"/>
       <c r="E47" s="34"/>
       <c r="F47" s="34"/>
       <c r="G47" s="34"/>
@@ -6406,15 +6415,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O99"/>
+  <dimension ref="A1:O100"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="2"/>
     <col min="2" max="2" width="12.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="15" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="29.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
@@ -6489,15 +6500,15 @@
       <c r="B4" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="58" t="s">
+      <c r="C4" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="62"/>
-      <c r="I4" s="59"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="64"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
@@ -6510,15 +6521,15 @@
       <c r="B5" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="58" t="s">
+      <c r="C5" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
-      <c r="H5" s="62"/>
-      <c r="I5" s="59"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="64"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -6531,15 +6542,15 @@
       <c r="B6" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="58" t="s">
+      <c r="C6" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="62"/>
-      <c r="E6" s="62"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="62"/>
-      <c r="H6" s="62"/>
-      <c r="I6" s="59"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="67"/>
+      <c r="H6" s="67"/>
+      <c r="I6" s="64"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -6552,15 +6563,15 @@
       <c r="B7" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="58" t="s">
+      <c r="C7" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="62"/>
-      <c r="H7" s="62"/>
-      <c r="I7" s="59"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="67"/>
+      <c r="I7" s="64"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -6625,19 +6636,19 @@
     </row>
     <row r="11" spans="1:15" ht="20" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="71" t="s">
+      <c r="B11" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="72"/>
+      <c r="C11" s="77"/>
       <c r="D11" s="44"/>
       <c r="E11" s="44"/>
       <c r="F11" s="44"/>
       <c r="G11" s="44"/>
       <c r="H11" s="44"/>
       <c r="I11" s="44"/>
-      <c r="J11" s="68"/>
-      <c r="K11" s="68"/>
-      <c r="L11" s="68"/>
+      <c r="J11" s="73"/>
+      <c r="K11" s="73"/>
+      <c r="L11" s="73"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
@@ -6666,11 +6677,11 @@
       <c r="I12" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="J12" s="69" t="s">
+      <c r="J12" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="K12" s="69"/>
-      <c r="L12" s="69"/>
+      <c r="K12" s="74"/>
+      <c r="L12" s="74"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
@@ -6699,11 +6710,11 @@
       <c r="I13" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="J13" s="63" t="s">
+      <c r="J13" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="K13" s="63"/>
-      <c r="L13" s="63"/>
+      <c r="K13" s="68"/>
+      <c r="L13" s="68"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
@@ -6715,7 +6726,7 @@
         <v>85</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>83</v>
+        <v>113</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>54</v>
@@ -6730,11 +6741,11 @@
       <c r="I14" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="J14" s="63" t="s">
+      <c r="J14" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="K14" s="63"/>
-      <c r="L14" s="63"/>
+      <c r="K14" s="68"/>
+      <c r="L14" s="68"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
@@ -6761,18 +6772,18 @@
       <c r="I15" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="J15" s="63" t="s">
+      <c r="J15" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="K15" s="63"/>
-      <c r="L15" s="63"/>
+      <c r="K15" s="68"/>
+      <c r="L15" s="68"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
     </row>
     <row r="16" spans="1:15" ht="20" customHeight="1">
       <c r="A16" s="1"/>
-      <c r="B16" s="43"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="14" t="s">
         <v>82</v>
       </c>
@@ -6794,125 +6805,127 @@
       <c r="I16" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="J16" s="63" t="s">
+      <c r="J16" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="K16" s="63"/>
-      <c r="L16" s="63"/>
+      <c r="K16" s="68"/>
+      <c r="L16" s="68"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
     </row>
     <row r="17" spans="1:15" ht="20" customHeight="1">
       <c r="A17" s="1"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="16"/>
-      <c r="L17" s="16"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F17" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H17" s="5">
+        <v>254</v>
+      </c>
+      <c r="I17" s="46" t="s">
+        <v>94</v>
+      </c>
+      <c r="J17" s="68" t="s">
+        <v>95</v>
+      </c>
+      <c r="K17" s="68"/>
+      <c r="L17" s="68"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
     </row>
-    <row r="18" spans="1:15" s="19" customFormat="1" ht="20" customHeight="1">
-      <c r="A18" s="11"/>
-      <c r="B18" s="73" t="s">
+    <row r="18" spans="1:15" ht="20" customHeight="1">
+      <c r="A18" s="1"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+    </row>
+    <row r="19" spans="1:15" s="19" customFormat="1" ht="20" customHeight="1">
+      <c r="A19" s="11"/>
+      <c r="B19" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="73"/>
-      <c r="D18" s="73"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="11"/>
-      <c r="M18" s="11"/>
-      <c r="N18" s="11"/>
-      <c r="O18" s="11"/>
-    </row>
-    <row r="19" spans="1:15" s="23" customFormat="1" ht="20" customHeight="1">
-      <c r="A19" s="21"/>
-      <c r="B19" s="64" t="s">
+      <c r="C19" s="78"/>
+      <c r="D19" s="78"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
+    </row>
+    <row r="20" spans="1:15" s="23" customFormat="1" ht="20" customHeight="1">
+      <c r="A20" s="21"/>
+      <c r="B20" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="65"/>
-      <c r="D19" s="65"/>
-      <c r="E19" s="66"/>
-      <c r="F19" s="52" t="s">
+      <c r="C20" s="70"/>
+      <c r="D20" s="70"/>
+      <c r="E20" s="71"/>
+      <c r="F20" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="G19" s="52" t="s">
+      <c r="G20" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="H19" s="52" t="s">
+      <c r="H20" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="I19" s="52" t="s">
+      <c r="I20" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="J19" s="52" t="s">
+      <c r="J20" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="K19" s="52" t="s">
+      <c r="K20" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="L19" s="52" t="s">
+      <c r="L20" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="M19" s="21"/>
-      <c r="N19" s="21"/>
-      <c r="O19" s="21"/>
-    </row>
-    <row r="20" spans="1:15" ht="20" customHeight="1">
-      <c r="A20" s="1"/>
-      <c r="B20" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="J20" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="K20" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="L20" s="3"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
+      <c r="M20" s="21"/>
+      <c r="N20" s="21"/>
+      <c r="O20" s="21"/>
     </row>
     <row r="21" spans="1:15" ht="20" customHeight="1">
       <c r="A21" s="1"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="D21" s="26"/>
+      <c r="B21" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
       <c r="E21" s="24"/>
-      <c r="F21" s="14" t="s">
-        <v>50</v>
+      <c r="F21" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>42</v>
@@ -6920,8 +6933,8 @@
       <c r="H21" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="I21" s="5">
-        <v>1</v>
+      <c r="I21" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="J21" s="5" t="s">
         <v>42</v>
@@ -6937,13 +6950,13 @@
     <row r="22" spans="1:15" ht="20" customHeight="1">
       <c r="A22" s="1"/>
       <c r="B22" s="13"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="25" t="s">
-        <v>53</v>
-      </c>
+      <c r="C22" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="26"/>
       <c r="E22" s="24"/>
       <c r="F22" s="14" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>42</v>
@@ -6960,7 +6973,7 @@
       <c r="K22" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="L22" s="28"/>
+      <c r="L22" s="3"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
@@ -6969,31 +6982,29 @@
       <c r="A23" s="1"/>
       <c r="B23" s="13"/>
       <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="29" t="s">
-        <v>46</v>
-      </c>
+      <c r="D23" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" s="24"/>
       <c r="F23" s="14" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H23" s="47" t="s">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="I23" s="5">
         <v>1</v>
       </c>
-      <c r="J23" s="5">
-        <v>3</v>
-      </c>
-      <c r="K23" s="5">
-        <v>3</v>
-      </c>
-      <c r="L23" s="3" t="s">
-        <v>27</v>
-      </c>
+      <c r="J23" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="L23" s="28"/>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
@@ -7003,11 +7014,11 @@
       <c r="B24" s="13"/>
       <c r="C24" s="27"/>
       <c r="D24" s="27"/>
-      <c r="E24" s="30" t="s">
-        <v>47</v>
+      <c r="E24" s="29" t="s">
+        <v>46</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G24" s="5" t="s">
         <v>26</v>
@@ -7019,13 +7030,13 @@
         <v>1</v>
       </c>
       <c r="J24" s="5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K24" s="5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
@@ -7033,17 +7044,17 @@
     </row>
     <row r="25" spans="1:15" ht="20" customHeight="1">
       <c r="A25" s="1"/>
-      <c r="B25" s="31"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="58" t="s">
-        <v>58</v>
-      </c>
-      <c r="E25" s="59"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="30" t="s">
+        <v>47</v>
+      </c>
       <c r="F25" s="14" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="H25" s="47" t="s">
         <v>41</v>
@@ -7051,39 +7062,53 @@
       <c r="I25" s="5">
         <v>1</v>
       </c>
-      <c r="J25" s="5" t="s">
-        <v>42</v>
+      <c r="J25" s="5">
+        <v>0</v>
       </c>
       <c r="K25" s="5">
-        <v>254</v>
-      </c>
-      <c r="L25" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
     </row>
     <row r="26" spans="1:15" ht="20" customHeight="1">
       <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="63" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" s="64"/>
+      <c r="F26" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H26" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="I26" s="5">
+        <v>1</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K26" s="5">
+        <v>254</v>
+      </c>
+      <c r="L26" s="3"/>
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
     </row>
     <row r="27" spans="1:15" ht="20" customHeight="1">
       <c r="A27" s="1"/>
-      <c r="B27" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -7100,7 +7125,9 @@
     </row>
     <row r="28" spans="1:15" ht="20" customHeight="1">
       <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
+      <c r="B28" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -7202,11 +7229,9 @@
     </row>
     <row r="34" spans="1:15" ht="20" customHeight="1">
       <c r="A34" s="1"/>
-      <c r="B34" s="73" t="s">
-        <v>31</v>
-      </c>
-      <c r="C34" s="73"/>
-      <c r="D34" s="73"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
@@ -7221,78 +7246,66 @@
     </row>
     <row r="35" spans="1:15" ht="20" customHeight="1">
       <c r="A35" s="1"/>
-      <c r="B35" s="64" t="s">
-        <v>14</v>
-      </c>
-      <c r="C35" s="65"/>
-      <c r="D35" s="65"/>
-      <c r="E35" s="66"/>
-      <c r="F35" s="52" t="s">
-        <v>21</v>
-      </c>
-      <c r="G35" s="52" t="s">
-        <v>15</v>
-      </c>
-      <c r="H35" s="52" t="s">
-        <v>16</v>
-      </c>
-      <c r="I35" s="52" t="s">
-        <v>24</v>
-      </c>
-      <c r="J35" s="52" t="s">
-        <v>17</v>
-      </c>
-      <c r="K35" s="52" t="s">
-        <v>18</v>
-      </c>
-      <c r="L35" s="52" t="s">
-        <v>20</v>
-      </c>
+      <c r="B35" s="78" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" s="78"/>
+      <c r="D35" s="78"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
     </row>
     <row r="36" spans="1:15" ht="20" customHeight="1">
       <c r="A36" s="1"/>
-      <c r="B36" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="24"/>
-      <c r="F36" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="G36" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="H36" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="I36" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="J36" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="K36" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="L36" s="3"/>
+      <c r="B36" s="69" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" s="70"/>
+      <c r="D36" s="70"/>
+      <c r="E36" s="71"/>
+      <c r="F36" s="52" t="s">
+        <v>21</v>
+      </c>
+      <c r="G36" s="52" t="s">
+        <v>15</v>
+      </c>
+      <c r="H36" s="52" t="s">
+        <v>16</v>
+      </c>
+      <c r="I36" s="52" t="s">
+        <v>24</v>
+      </c>
+      <c r="J36" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="K36" s="52" t="s">
+        <v>18</v>
+      </c>
+      <c r="L36" s="52" t="s">
+        <v>20</v>
+      </c>
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
     </row>
     <row r="37" spans="1:15" ht="20" customHeight="1">
-      <c r="A37" s="4"/>
-      <c r="B37" s="13"/>
-      <c r="C37" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="D37" s="26"/>
+      <c r="A37" s="1"/>
+      <c r="B37" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="C37" s="20"/>
+      <c r="D37" s="20"/>
       <c r="E37" s="24"/>
-      <c r="F37" s="14" t="s">
-        <v>50</v>
+      <c r="F37" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>42</v>
@@ -7317,13 +7330,13 @@
     <row r="38" spans="1:15" ht="20" customHeight="1">
       <c r="A38" s="4"/>
       <c r="B38" s="13"/>
-      <c r="C38" s="27"/>
-      <c r="D38" s="25" t="s">
-        <v>53</v>
-      </c>
+      <c r="C38" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="D38" s="26"/>
       <c r="E38" s="24"/>
       <c r="F38" s="14" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="G38" s="5" t="s">
         <v>42</v>
@@ -7340,7 +7353,7 @@
       <c r="K38" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="L38" s="28"/>
+      <c r="L38" s="3"/>
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
@@ -7349,45 +7362,43 @@
       <c r="A39" s="4"/>
       <c r="B39" s="13"/>
       <c r="C39" s="27"/>
-      <c r="D39" s="27"/>
-      <c r="E39" s="29" t="s">
-        <v>46</v>
-      </c>
+      <c r="D39" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="E39" s="24"/>
       <c r="F39" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H39" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="I39" s="5">
-        <v>1</v>
-      </c>
-      <c r="J39" s="5">
-        <v>3</v>
-      </c>
-      <c r="K39" s="5">
-        <v>3</v>
-      </c>
-      <c r="L39" s="3" t="s">
-        <v>62</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J39" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K39" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="L39" s="28"/>
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
       <c r="O39" s="1"/>
     </row>
-    <row r="40" spans="1:15" s="37" customFormat="1" ht="20" customHeight="1">
+    <row r="40" spans="1:15" ht="20" customHeight="1">
       <c r="A40" s="4"/>
-      <c r="B40" s="31"/>
-      <c r="C40" s="32"/>
-      <c r="D40" s="32"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
       <c r="E40" s="29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F40" s="14" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G40" s="3" t="s">
         <v>26</v>
@@ -7399,42 +7410,56 @@
         <v>1</v>
       </c>
       <c r="J40" s="5">
+        <v>3</v>
+      </c>
+      <c r="K40" s="5">
+        <v>3</v>
+      </c>
+      <c r="L40" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
+      <c r="O40" s="1"/>
+    </row>
+    <row r="41" spans="1:15" s="37" customFormat="1" ht="20" customHeight="1">
+      <c r="A41" s="4"/>
+      <c r="B41" s="31"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="32"/>
+      <c r="E41" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="F41" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H41" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="I41" s="5">
+        <v>1</v>
+      </c>
+      <c r="J41" s="5">
         <v>0</v>
       </c>
-      <c r="K40" s="5">
+      <c r="K41" s="5">
         <v>254</v>
       </c>
-      <c r="L40" s="3" t="s">
+      <c r="L41" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="M40" s="4"/>
-      <c r="N40" s="4"/>
-      <c r="O40" s="4"/>
-    </row>
-    <row r="41" spans="1:15" ht="20" customHeight="1">
-      <c r="A41" s="4"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="1"/>
-      <c r="L41" s="1"/>
-      <c r="M41" s="1"/>
-      <c r="N41" s="1"/>
-      <c r="O41" s="1"/>
+      <c r="M41" s="4"/>
+      <c r="N41" s="4"/>
+      <c r="O41" s="4"/>
     </row>
     <row r="42" spans="1:15" ht="20" customHeight="1">
-      <c r="A42" s="1"/>
-      <c r="B42" s="67" t="s">
-        <v>33</v>
-      </c>
-      <c r="C42" s="67"/>
-      <c r="D42" s="67"/>
+      <c r="A42" s="4"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
@@ -7449,13 +7474,11 @@
     </row>
     <row r="43" spans="1:15" ht="20" customHeight="1">
       <c r="A43" s="1"/>
-      <c r="B43" s="54">
-        <v>200</v>
-      </c>
-      <c r="C43" s="58" t="s">
-        <v>34</v>
-      </c>
-      <c r="D43" s="59"/>
+      <c r="B43" s="72" t="s">
+        <v>33</v>
+      </c>
+      <c r="C43" s="72"/>
+      <c r="D43" s="72"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
@@ -7471,12 +7494,12 @@
     <row r="44" spans="1:15" ht="20" customHeight="1">
       <c r="A44" s="1"/>
       <c r="B44" s="54">
-        <v>401</v>
-      </c>
-      <c r="C44" s="58" t="s">
-        <v>67</v>
-      </c>
-      <c r="D44" s="59"/>
+        <v>200</v>
+      </c>
+      <c r="C44" s="63" t="s">
+        <v>34</v>
+      </c>
+      <c r="D44" s="64"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
@@ -7492,12 +7515,12 @@
     <row r="45" spans="1:15" ht="20" customHeight="1">
       <c r="A45" s="1"/>
       <c r="B45" s="54">
-        <v>402</v>
-      </c>
-      <c r="C45" s="58" t="s">
-        <v>78</v>
-      </c>
-      <c r="D45" s="59"/>
+        <v>401</v>
+      </c>
+      <c r="C45" s="63" t="s">
+        <v>67</v>
+      </c>
+      <c r="D45" s="64"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
@@ -7510,115 +7533,119 @@
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
     </row>
-    <row r="46" spans="1:15" s="35" customFormat="1" ht="20" customHeight="1">
+    <row r="46" spans="1:15" ht="20" customHeight="1">
       <c r="A46" s="1"/>
       <c r="B46" s="54">
+        <v>402</v>
+      </c>
+      <c r="C46" s="63" t="s">
+        <v>78</v>
+      </c>
+      <c r="D46" s="64"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
+      <c r="L46" s="1"/>
+      <c r="M46" s="1"/>
+      <c r="N46" s="1"/>
+      <c r="O46" s="1"/>
+    </row>
+    <row r="47" spans="1:15" s="35" customFormat="1" ht="20" customHeight="1">
+      <c r="A47" s="1"/>
+      <c r="B47" s="54">
         <v>403</v>
       </c>
-      <c r="C46" s="58" t="s">
+      <c r="C47" s="63" t="s">
         <v>79</v>
       </c>
-      <c r="D46" s="59"/>
-      <c r="E46" s="34"/>
-      <c r="F46" s="34"/>
-      <c r="G46" s="34"/>
-      <c r="H46" s="34"/>
-      <c r="I46" s="34"/>
-      <c r="J46" s="34"/>
-      <c r="K46" s="34"/>
-      <c r="L46" s="34"/>
-      <c r="M46" s="34"/>
-      <c r="N46" s="34"/>
-      <c r="O46" s="34"/>
-    </row>
-    <row r="47" spans="1:15" ht="20" customHeight="1">
-      <c r="A47" s="34"/>
-      <c r="B47" s="39">
+      <c r="D47" s="64"/>
+      <c r="E47" s="34"/>
+      <c r="F47" s="34"/>
+      <c r="G47" s="34"/>
+      <c r="H47" s="34"/>
+      <c r="I47" s="34"/>
+      <c r="J47" s="34"/>
+      <c r="K47" s="34"/>
+      <c r="L47" s="34"/>
+      <c r="M47" s="34"/>
+      <c r="N47" s="34"/>
+      <c r="O47" s="34"/>
+    </row>
+    <row r="48" spans="1:15" ht="20" customHeight="1">
+      <c r="A48" s="34"/>
+      <c r="B48" s="39">
         <v>500</v>
       </c>
-      <c r="C47" s="60" t="s">
+      <c r="C48" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="D47" s="61"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
-      <c r="J47" s="1"/>
-      <c r="K47" s="1"/>
-      <c r="L47" s="1"/>
-      <c r="M47" s="1"/>
-      <c r="N47" s="1"/>
-      <c r="O47" s="1"/>
-    </row>
-    <row r="48" spans="1:15" s="35" customFormat="1" ht="20" customHeight="1">
-      <c r="A48" s="34"/>
-      <c r="B48" s="34"/>
-      <c r="C48" s="34"/>
-      <c r="D48" s="34"/>
-      <c r="E48" s="34"/>
-      <c r="F48" s="34"/>
-      <c r="G48" s="34"/>
-      <c r="H48" s="34"/>
-      <c r="I48" s="34"/>
-      <c r="J48" s="34"/>
-      <c r="K48" s="34"/>
-      <c r="L48" s="34"/>
-      <c r="M48" s="34"/>
-      <c r="N48" s="34"/>
-      <c r="O48" s="34"/>
-    </row>
-    <row r="49" spans="1:15" ht="20" customHeight="1">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
-      <c r="I49" s="1"/>
-      <c r="J49" s="1"/>
-      <c r="K49" s="1"/>
-      <c r="L49" s="1"/>
-      <c r="M49" s="1"/>
-      <c r="N49" s="1"/>
-      <c r="O49" s="1"/>
-    </row>
-    <row r="50" spans="1:15" s="35" customFormat="1" ht="20" customHeight="1">
-      <c r="A50" s="34"/>
-      <c r="B50" s="34"/>
-      <c r="C50" s="34"/>
-      <c r="D50" s="34"/>
-      <c r="E50" s="34"/>
-      <c r="F50" s="34"/>
-      <c r="G50" s="34"/>
-      <c r="H50" s="34"/>
-      <c r="I50" s="34"/>
-      <c r="J50" s="34"/>
-      <c r="K50" s="34"/>
-      <c r="L50" s="34"/>
-      <c r="M50" s="34"/>
-      <c r="N50" s="34"/>
-      <c r="O50" s="34"/>
-    </row>
-    <row r="51" spans="1:15" ht="20" customHeight="1">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
-      <c r="H51" s="1"/>
-      <c r="I51" s="1"/>
-      <c r="J51" s="1"/>
-      <c r="K51" s="1"/>
-      <c r="L51" s="1"/>
-      <c r="M51" s="1"/>
-      <c r="N51" s="1"/>
-      <c r="O51" s="1"/>
+      <c r="D48" s="66"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
+      <c r="L48" s="1"/>
+      <c r="M48" s="1"/>
+      <c r="N48" s="1"/>
+      <c r="O48" s="1"/>
+    </row>
+    <row r="49" spans="1:15" s="35" customFormat="1" ht="20" customHeight="1">
+      <c r="A49" s="34"/>
+      <c r="B49" s="34"/>
+      <c r="C49" s="34"/>
+      <c r="D49" s="34"/>
+      <c r="E49" s="34"/>
+      <c r="F49" s="34"/>
+      <c r="G49" s="34"/>
+      <c r="H49" s="34"/>
+      <c r="I49" s="34"/>
+      <c r="J49" s="34"/>
+      <c r="K49" s="34"/>
+      <c r="L49" s="34"/>
+      <c r="M49" s="34"/>
+      <c r="N49" s="34"/>
+      <c r="O49" s="34"/>
+    </row>
+    <row r="50" spans="1:15" ht="20" customHeight="1">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
+      <c r="L50" s="1"/>
+      <c r="M50" s="1"/>
+      <c r="N50" s="1"/>
+      <c r="O50" s="1"/>
+    </row>
+    <row r="51" spans="1:15" s="35" customFormat="1" ht="20" customHeight="1">
+      <c r="A51" s="34"/>
+      <c r="B51" s="34"/>
+      <c r="C51" s="34"/>
+      <c r="D51" s="34"/>
+      <c r="E51" s="34"/>
+      <c r="F51" s="34"/>
+      <c r="G51" s="34"/>
+      <c r="H51" s="34"/>
+      <c r="I51" s="34"/>
+      <c r="J51" s="34"/>
+      <c r="K51" s="34"/>
+      <c r="L51" s="34"/>
+      <c r="M51" s="34"/>
+      <c r="N51" s="34"/>
+      <c r="O51" s="34"/>
     </row>
     <row r="52" spans="1:15" ht="20" customHeight="1">
       <c r="A52" s="1"/>
@@ -8420,33 +8447,52 @@
       <c r="O98" s="1"/>
     </row>
     <row r="99" spans="1:15" ht="20" customHeight="1">
-      <c r="A99" s="36"/>
-      <c r="B99" s="36"/>
-      <c r="C99" s="36"/>
-      <c r="D99" s="36"/>
-      <c r="E99" s="36"/>
-      <c r="F99" s="36"/>
-      <c r="G99" s="36"/>
-      <c r="H99" s="36"/>
-      <c r="I99" s="36"/>
-      <c r="J99" s="36"/>
-      <c r="K99" s="36"/>
-      <c r="L99" s="36"/>
-      <c r="M99" s="36"/>
-      <c r="N99" s="36"/>
-      <c r="O99" s="36"/>
+      <c r="A99" s="1"/>
+      <c r="B99" s="1"/>
+      <c r="C99" s="1"/>
+      <c r="D99" s="1"/>
+      <c r="E99" s="1"/>
+      <c r="F99" s="1"/>
+      <c r="G99" s="1"/>
+      <c r="H99" s="1"/>
+      <c r="I99" s="1"/>
+      <c r="J99" s="1"/>
+      <c r="K99" s="1"/>
+      <c r="L99" s="1"/>
+      <c r="M99" s="1"/>
+      <c r="N99" s="1"/>
+      <c r="O99" s="1"/>
+    </row>
+    <row r="100" spans="1:15" ht="20" customHeight="1">
+      <c r="A100" s="36"/>
+      <c r="B100" s="36"/>
+      <c r="C100" s="36"/>
+      <c r="D100" s="36"/>
+      <c r="E100" s="36"/>
+      <c r="F100" s="36"/>
+      <c r="G100" s="36"/>
+      <c r="H100" s="36"/>
+      <c r="I100" s="36"/>
+      <c r="J100" s="36"/>
+      <c r="K100" s="36"/>
+      <c r="L100" s="36"/>
+      <c r="M100" s="36"/>
+      <c r="N100" s="36"/>
+      <c r="O100" s="36"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="B35:E35"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="C43:D43"/>
+  <mergeCells count="23">
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="B36:E36"/>
+    <mergeCell ref="B43:D43"/>
     <mergeCell ref="C44:D44"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="J17:L17"/>
+    <mergeCell ref="C46:D46"/>
     <mergeCell ref="J11:L11"/>
-    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
     <mergeCell ref="C4:I4"/>
     <mergeCell ref="C5:I5"/>
     <mergeCell ref="C6:I6"/>
@@ -8455,18 +8501,18 @@
     <mergeCell ref="J12:L12"/>
     <mergeCell ref="J13:L13"/>
     <mergeCell ref="J16:L16"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="C47:D47"/>
     <mergeCell ref="J15:L15"/>
-    <mergeCell ref="J14:L14"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I13" r:id="rId1"/>
+    <hyperlink ref="I17" r:id="rId2" display="foo@mulodo.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -8479,8 +8525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O100"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A14" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -8562,15 +8608,15 @@
       <c r="B4" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="58" t="s">
+      <c r="C4" s="63" t="s">
         <v>90</v>
       </c>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="62"/>
-      <c r="I4" s="59"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="64"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
@@ -8583,15 +8629,15 @@
       <c r="B5" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="58" t="s">
-        <v>104</v>
-      </c>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
-      <c r="H5" s="62"/>
-      <c r="I5" s="59"/>
+      <c r="C5" s="63" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="64"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -8604,15 +8650,15 @@
       <c r="B6" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="58" t="s">
+      <c r="C6" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="62"/>
-      <c r="E6" s="62"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="62"/>
-      <c r="H6" s="62"/>
-      <c r="I6" s="59"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="67"/>
+      <c r="H6" s="67"/>
+      <c r="I6" s="64"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -8625,15 +8671,15 @@
       <c r="B7" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="58" t="s">
+      <c r="C7" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="62"/>
-      <c r="H7" s="62"/>
-      <c r="I7" s="59"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="67"/>
+      <c r="I7" s="64"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -8698,19 +8744,19 @@
     </row>
     <row r="11" spans="1:15" ht="20" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="71" t="s">
+      <c r="B11" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="72"/>
+      <c r="C11" s="77"/>
       <c r="D11" s="44"/>
       <c r="E11" s="44"/>
       <c r="F11" s="44"/>
       <c r="G11" s="44"/>
       <c r="H11" s="44"/>
       <c r="I11" s="44"/>
-      <c r="J11" s="68"/>
-      <c r="K11" s="68"/>
-      <c r="L11" s="68"/>
+      <c r="J11" s="73"/>
+      <c r="K11" s="73"/>
+      <c r="L11" s="73"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
@@ -8739,11 +8785,11 @@
       <c r="I12" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="J12" s="69" t="s">
+      <c r="J12" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="K12" s="69"/>
-      <c r="L12" s="69"/>
+      <c r="K12" s="74"/>
+      <c r="L12" s="74"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
@@ -8772,11 +8818,11 @@
       <c r="I13" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="J13" s="63" t="s">
+      <c r="J13" s="68" t="s">
         <v>95</v>
       </c>
-      <c r="K13" s="63"/>
-      <c r="L13" s="63"/>
+      <c r="K13" s="68"/>
+      <c r="L13" s="68"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
@@ -8805,11 +8851,11 @@
       <c r="I14" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="J14" s="58" t="s">
-        <v>105</v>
-      </c>
-      <c r="K14" s="62"/>
-      <c r="L14" s="59"/>
+      <c r="J14" s="63" t="s">
+        <v>104</v>
+      </c>
+      <c r="K14" s="67"/>
+      <c r="L14" s="64"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
@@ -8833,25 +8879,25 @@
       <c r="H15" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="I15" s="74">
+      <c r="I15" s="58">
         <v>5</v>
       </c>
-      <c r="J15" s="75" t="s">
-        <v>106</v>
-      </c>
-      <c r="K15" s="76"/>
-      <c r="L15" s="77"/>
+      <c r="J15" s="59" t="s">
+        <v>105</v>
+      </c>
+      <c r="K15" s="60"/>
+      <c r="L15" s="61"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
     </row>
     <row r="16" spans="1:15" s="19" customFormat="1" ht="20" customHeight="1">
       <c r="A16" s="11"/>
-      <c r="B16" s="70" t="s">
+      <c r="B16" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="70"/>
-      <c r="D16" s="70"/>
+      <c r="C16" s="75"/>
+      <c r="D16" s="75"/>
       <c r="E16" s="17"/>
       <c r="F16" s="18"/>
       <c r="G16" s="17"/>
@@ -8866,12 +8912,12 @@
     </row>
     <row r="17" spans="1:15" s="23" customFormat="1" ht="20" customHeight="1">
       <c r="A17" s="21"/>
-      <c r="B17" s="64" t="s">
+      <c r="B17" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="65"/>
-      <c r="D17" s="65"/>
-      <c r="E17" s="66"/>
+      <c r="C17" s="70"/>
+      <c r="D17" s="70"/>
+      <c r="E17" s="71"/>
       <c r="F17" s="56" t="s">
         <v>21</v>
       </c>
@@ -9061,7 +9107,7 @@
       <c r="B23" s="13"/>
       <c r="C23" s="27"/>
       <c r="D23" s="57" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E23" s="24"/>
       <c r="F23" s="14" t="s">
@@ -9092,11 +9138,11 @@
       <c r="B24" s="13"/>
       <c r="C24" s="27"/>
       <c r="D24" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E24" s="24"/>
       <c r="F24" s="14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G24" s="5" t="s">
         <v>42</v>
@@ -9124,10 +9170,10 @@
       <c r="C25" s="27"/>
       <c r="D25" s="27"/>
       <c r="E25" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="F25" s="14" t="s">
         <v>109</v>
-      </c>
-      <c r="F25" s="14" t="s">
-        <v>110</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>103</v>
@@ -9153,7 +9199,7 @@
       <c r="A26" s="1"/>
       <c r="B26" s="31"/>
       <c r="C26" s="32"/>
-      <c r="D26" s="78"/>
+      <c r="D26" s="62"/>
       <c r="E26" s="29" t="s">
         <v>100</v>
       </c>
@@ -9320,11 +9366,11 @@
     </row>
     <row r="35" spans="1:15" ht="20" customHeight="1">
       <c r="A35" s="1"/>
-      <c r="B35" s="73" t="s">
+      <c r="B35" s="78" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="73"/>
-      <c r="D35" s="73"/>
+      <c r="C35" s="78"/>
+      <c r="D35" s="78"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
@@ -9339,12 +9385,12 @@
     </row>
     <row r="36" spans="1:15" ht="20" customHeight="1">
       <c r="A36" s="1"/>
-      <c r="B36" s="64" t="s">
+      <c r="B36" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="C36" s="65"/>
-      <c r="D36" s="65"/>
-      <c r="E36" s="66"/>
+      <c r="C36" s="70"/>
+      <c r="D36" s="70"/>
+      <c r="E36" s="71"/>
       <c r="F36" s="56" t="s">
         <v>21</v>
       </c>
@@ -9548,11 +9594,11 @@
     </row>
     <row r="43" spans="1:15" ht="20" customHeight="1">
       <c r="A43" s="1"/>
-      <c r="B43" s="73" t="s">
+      <c r="B43" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="C43" s="73"/>
-      <c r="D43" s="73"/>
+      <c r="C43" s="78"/>
+      <c r="D43" s="78"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
@@ -9570,10 +9616,10 @@
       <c r="B44" s="55">
         <v>200</v>
       </c>
-      <c r="C44" s="58" t="s">
+      <c r="C44" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="D44" s="59"/>
+      <c r="D44" s="64"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
@@ -9591,10 +9637,10 @@
       <c r="B45" s="55">
         <v>401</v>
       </c>
-      <c r="C45" s="58" t="s">
+      <c r="C45" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="D45" s="59"/>
+      <c r="D45" s="64"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
@@ -9612,10 +9658,10 @@
       <c r="B46" s="55">
         <v>402</v>
       </c>
-      <c r="C46" s="58" t="s">
+      <c r="C46" s="63" t="s">
         <v>68</v>
       </c>
-      <c r="D46" s="59"/>
+      <c r="D46" s="64"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
@@ -9633,10 +9679,10 @@
       <c r="B47" s="39">
         <v>500</v>
       </c>
-      <c r="C47" s="60" t="s">
+      <c r="C47" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="D47" s="61"/>
+      <c r="D47" s="66"/>
       <c r="E47" s="34"/>
       <c r="F47" s="34"/>
       <c r="G47" s="34"/>

</xml_diff>